<commit_message>
Fixed missing rows (passes first assertion)
</commit_message>
<xml_diff>
--- a/variable-dosing_7119.xlsx
+++ b/variable-dosing_7119.xlsx
@@ -5,12 +5,12 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaston\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaston\Desktop\GBM-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E2C051F9-10CB-4C67-A376-D9B8C8B14451}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2AAE1C1D-7666-465C-9606-5BE4AFC26C75}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="677" uniqueCount="164">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="687" uniqueCount="164">
   <si>
     <t>Phase</t>
   </si>
@@ -1235,31 +1235,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color theme="9" tint="0.39997558519241921"/>
@@ -1416,6 +1391,31 @@
         <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
         <u/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
@@ -1481,8 +1481,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2A8E3CB-1AFB-479A-A935-6E3A8A8C1E2A}" name="Table2" displayName="Table2" ref="A1:AN45" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:AN45" xr:uid="{337B527E-CC89-49CB-B8CF-29513C2E5B70}"/>
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2A8E3CB-1AFB-479A-A935-6E3A8A8C1E2A}" name="Table2" displayName="Table2" ref="A1:AN47" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:AN47" xr:uid="{337B527E-CC89-49CB-B8CF-29513C2E5B70}"/>
   <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{04959165-9B47-46FC-95B1-128303AC6772}" name="NCT"/>
     <tableColumn id="2" xr3:uid="{749B59FF-4A21-40FD-8008-2136ADB4D3D2}" name="Arm"/>
@@ -1543,14 +1543,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7B3D4233-F20E-48BF-9756-1CD7CC13A260}" name="Table4" displayName="Table4" ref="A1:E2" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7B3D4233-F20E-48BF-9756-1CD7CC13A260}" name="Table4" displayName="Table4" ref="A1:E2" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:E2" xr:uid="{C91D0DA2-D727-4E0F-8EC4-17B25C4E8387}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{E4577221-1973-4BCF-BAF7-1AB70117714D}" name="NCT"/>
     <tableColumn id="2" xr3:uid="{EA872DFA-99BE-4320-90D2-4CF33088C1B5}" name="Arm"/>
-    <tableColumn id="3" xr3:uid="{30298370-E7DF-4944-A120-B51B0265395A}" name="Neo Drug" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{7E187766-C32E-4BD3-80B1-4B9D8AA592BE}" name="Neo Drug Dosage" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{54CEE142-B286-436E-BD32-02E0329ABA44}" name="Neo Drug Dosage Unit" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{30298370-E7DF-4944-A120-B51B0265395A}" name="Neo Drug" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{7E187766-C32E-4BD3-80B1-4B9D8AA592BE}" name="Neo Drug Dosage" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{54CEE142-B286-436E-BD32-02E0329ABA44}" name="Neo Drug Dosage Unit" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1573,7 +1573,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{15337EB3-855F-4F50-B6E4-CECAA2CCDEF0}" name="Table6" displayName="Table6" ref="A1:E23" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1">
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{15337EB3-855F-4F50-B6E4-CECAA2CCDEF0}" name="Table6" displayName="Table6" ref="A1:E23" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="0">
   <autoFilter ref="A1:E23" xr:uid="{DB024295-AB18-4A25-866D-45881406AE0C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D7325FB9-74D1-4609-855A-27A9CEC4B977}" name="NCT"/>
@@ -1885,8 +1885,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2099,10 +2099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AN45"/>
+  <dimension ref="A1:AN47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4965,6 +4965,133 @@
         <v>0</v>
       </c>
     </row>
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>16</v>
+      </c>
+      <c r="B46" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46">
+        <v>9</v>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" t="b">
+        <v>0</v>
+      </c>
+      <c r="X46" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y46" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB46">
+        <v>20</v>
+      </c>
+      <c r="AC46" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH46" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI46">
+        <v>75</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>16</v>
+      </c>
+      <c r="B47" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47">
+        <v>38</v>
+      </c>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" t="b">
+        <v>0</v>
+      </c>
+      <c r="X47" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y47" t="b">
+        <v>1</v>
+      </c>
+      <c r="Z47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB47">
+        <v>40</v>
+      </c>
+      <c r="AC47" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH47" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI47">
+        <v>150</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN47">
+        <v>4.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4977,8 +5104,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7336,7 +7463,7 @@
     <col min="5" max="5" width="19.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>

</xml_diff>

<commit_message>
Added "% Serious AE" &
</commit_message>
<xml_diff>
--- a/variable-dosing_7119.xlsx
+++ b/variable-dosing_7119.xlsx
@@ -5,10 +5,10 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaston\Desktop\GBM-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaston\Desktop\GBM-master\GBM-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2AAE1C1D-7666-465C-9606-5BE4AFC26C75}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0BD252BF-9BA7-4783-94E5-493B11977E6C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="687" uniqueCount="164">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="689" uniqueCount="166">
   <si>
     <t>Phase</t>
   </si>
@@ -522,12 +522,21 @@
   </si>
   <si>
     <t>Dropouts</t>
+  </si>
+  <si>
+    <t>% Serious AE</t>
+  </si>
+  <si>
+    <t>% Non Serious AE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1104,7 +1113,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1147,8 +1156,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1188,8 +1198,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1229,6 +1243,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1481,12 +1496,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2A8E3CB-1AFB-479A-A935-6E3A8A8C1E2A}" name="Table2" displayName="Table2" ref="A1:AN47" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:AN47" xr:uid="{337B527E-CC89-49CB-B8CF-29513C2E5B70}"/>
-  <tableColumns count="40">
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2A8E3CB-1AFB-479A-A935-6E3A8A8C1E2A}" name="Table2" displayName="Table2" ref="A1:AP47" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A1:AP47" xr:uid="{337B527E-CC89-49CB-B8CF-29513C2E5B70}"/>
+  <tableColumns count="42">
     <tableColumn id="1" xr3:uid="{04959165-9B47-46FC-95B1-128303AC6772}" name="NCT"/>
     <tableColumn id="2" xr3:uid="{749B59FF-4A21-40FD-8008-2136ADB4D3D2}" name="Arm"/>
     <tableColumn id="3" xr3:uid="{812D4910-70D1-4BB6-9392-9EE81E6B607E}" name="Enrollment"/>
+    <tableColumn id="8" xr3:uid="{CFE8251D-EE80-4F6B-B4D7-9778DA29951D}" name="% Serious AE"/>
+    <tableColumn id="7" xr3:uid="{1BA1B69D-E3FC-4024-A433-38F8B81A1455}" name="% Non Serious AE"/>
     <tableColumn id="4" xr3:uid="{63022E9F-2D81-498D-8C05-BF852023D8B8}" name="Radiation"/>
     <tableColumn id="5" xr3:uid="{869510A2-1CE0-437C-9ED4-65B04D4A1360}" name="Randomized"/>
     <tableColumn id="10" xr3:uid="{03B678CC-1932-4A2C-AAB0-73B5893DD292}" name="Surgery"/>
@@ -1886,7 +1903,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2099,55 +2116,57 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AN47"/>
+  <dimension ref="A1:AP47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="75.75" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
-    <col min="6" max="6" width="12.75" customWidth="1"/>
-    <col min="7" max="7" width="13.75" customWidth="1"/>
-    <col min="8" max="8" width="27.75" customWidth="1"/>
-    <col min="9" max="9" width="20.625" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
-    <col min="11" max="11" width="20.75" customWidth="1"/>
-    <col min="12" max="12" width="24.125" customWidth="1"/>
+    <col min="4" max="4" width="15.25" customWidth="1"/>
+    <col min="5" max="5" width="17.375" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="9" max="9" width="13.75" customWidth="1"/>
+    <col min="10" max="10" width="27.75" customWidth="1"/>
+    <col min="11" max="11" width="20.625" customWidth="1"/>
+    <col min="12" max="12" width="13.5" customWidth="1"/>
     <col min="13" max="13" width="20.75" customWidth="1"/>
-    <col min="14" max="14" width="23.375" customWidth="1"/>
-    <col min="15" max="15" width="15" customWidth="1"/>
-    <col min="16" max="16" width="20.875" customWidth="1"/>
-    <col min="17" max="17" width="24.75" customWidth="1"/>
-    <col min="18" max="18" width="19.625" customWidth="1"/>
-    <col min="19" max="19" width="28.75" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="21" width="20.875" customWidth="1"/>
-    <col min="22" max="22" width="24.75" customWidth="1"/>
-    <col min="23" max="23" width="19.625" customWidth="1"/>
-    <col min="24" max="24" width="28.75" customWidth="1"/>
-    <col min="27" max="27" width="11.875" customWidth="1"/>
-    <col min="28" max="28" width="16.125" customWidth="1"/>
-    <col min="29" max="29" width="20.375" customWidth="1"/>
-    <col min="30" max="30" width="24.125" customWidth="1"/>
-    <col min="31" max="31" width="20.75" customWidth="1"/>
-    <col min="32" max="32" width="29.875" customWidth="1"/>
-    <col min="33" max="33" width="13.25" customWidth="1"/>
-    <col min="34" max="34" width="22.375" customWidth="1"/>
-    <col min="35" max="35" width="16.125" customWidth="1"/>
-    <col min="36" max="36" width="22.875" customWidth="1"/>
-    <col min="37" max="37" width="28.5" customWidth="1"/>
-    <col min="38" max="38" width="20.375" customWidth="1"/>
-    <col min="39" max="39" width="29.875" customWidth="1"/>
-    <col min="40" max="40" width="12.125" customWidth="1"/>
-    <col min="41" max="41" width="22.375" customWidth="1"/>
+    <col min="14" max="14" width="24.125" customWidth="1"/>
+    <col min="15" max="15" width="20.75" customWidth="1"/>
+    <col min="16" max="16" width="23.375" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="20.875" customWidth="1"/>
+    <col min="19" max="19" width="24.75" customWidth="1"/>
+    <col min="20" max="20" width="19.625" customWidth="1"/>
+    <col min="21" max="21" width="28.75" customWidth="1"/>
+    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="20.875" customWidth="1"/>
+    <col min="24" max="24" width="24.75" customWidth="1"/>
+    <col min="25" max="25" width="19.625" customWidth="1"/>
+    <col min="26" max="26" width="28.75" customWidth="1"/>
+    <col min="29" max="29" width="11.875" customWidth="1"/>
+    <col min="30" max="30" width="16.125" customWidth="1"/>
+    <col min="31" max="31" width="20.375" customWidth="1"/>
+    <col min="32" max="32" width="24.125" customWidth="1"/>
+    <col min="33" max="33" width="20.75" customWidth="1"/>
+    <col min="34" max="34" width="29.875" customWidth="1"/>
+    <col min="35" max="35" width="13.25" customWidth="1"/>
+    <col min="36" max="36" width="22.375" customWidth="1"/>
+    <col min="37" max="37" width="16.125" customWidth="1"/>
+    <col min="38" max="38" width="22.875" customWidth="1"/>
+    <col min="39" max="39" width="28.5" customWidth="1"/>
+    <col min="40" max="40" width="20.375" customWidth="1"/>
+    <col min="41" max="41" width="29.875" customWidth="1"/>
+    <col min="42" max="42" width="12.125" customWidth="1"/>
+    <col min="43" max="43" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -2158,118 +2177,124 @@
         <v>162</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="Z1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="AA1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AD1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AE1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AF1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AG1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AH1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AL1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AM1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AN1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AO1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AP1" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2279,71 +2304,77 @@
       <c r="C2">
         <v>122</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
+      <c r="D2" s="21">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="E2" s="21">
+        <v>0.8992</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>52</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>10</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>54</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>125</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>55</v>
       </c>
-      <c r="V2" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2">
+      <c r="X2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y2">
         <v>1.5</v>
       </c>
-      <c r="X2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y2" t="b">
-        <v>0</v>
-      </c>
       <c r="Z2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP2">
         <v>16.64</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2353,11 +2384,11 @@
       <c r="C3">
         <v>60</v>
       </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
+      <c r="D3" s="21">
+        <v>0.83640000000000003</v>
+      </c>
+      <c r="E3" s="21">
+        <v>0.67720000000000002</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
@@ -2366,34 +2397,40 @@
         <v>1</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>175</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>55</v>
       </c>
-      <c r="X3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="b">
-        <v>0</v>
-      </c>
       <c r="Z3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP3">
         <v>17.3</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2403,23 +2440,27 @@
       <c r="C4">
         <v>131</v>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
+      <c r="D4" s="24">
+        <v>0.42970000000000003</v>
+      </c>
+      <c r="E4" s="24">
+        <v>0.96879999999999999</v>
       </c>
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
@@ -2433,43 +2474,45 @@
       <c r="U4" s="11"/>
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
-      <c r="X4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="11" t="s">
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AD4" s="11">
         <v>30</v>
       </c>
-      <c r="AC4" s="11" t="s">
+      <c r="AE4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
+      <c r="AF4" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
       <c r="AI4" s="11"/>
       <c r="AJ4" s="11"/>
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
-      <c r="AM4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="11">
+      <c r="AM4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -2479,62 +2522,68 @@
       <c r="C5">
         <v>129</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
+      <c r="D5" s="24">
+        <v>0.3659</v>
+      </c>
+      <c r="E5" s="24">
+        <v>0.97560000000000002</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="X5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="11" t="s">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AB5">
+      <c r="AD5">
         <v>20</v>
       </c>
-      <c r="AC5" s="11" t="s">
+      <c r="AE5" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AD5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH5" t="s">
+      <c r="AF5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>69</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>110</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AL5" t="s">
         <v>55</v>
       </c>
-      <c r="AK5" t="b">
-        <v>0</v>
-      </c>
       <c r="AM5" t="b">
         <v>0</v>
       </c>
-      <c r="AN5">
+      <c r="AO5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP5">
         <v>9.4</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -2544,62 +2593,68 @@
       <c r="C6">
         <v>65</v>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
+      <c r="D6" s="24">
+        <v>0.40629999999999999</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0.95309999999999995</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="X6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="s">
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="s">
         <v>69</v>
       </c>
-      <c r="AB6">
+      <c r="AD6">
         <v>110</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AE6" t="s">
         <v>55</v>
       </c>
-      <c r="AD6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH6" t="s">
+      <c r="AF6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>71</v>
       </c>
-      <c r="AI6">
+      <c r="AK6">
         <v>20</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AL6" t="s">
         <v>65</v>
       </c>
-      <c r="AK6" t="b">
-        <v>0</v>
-      </c>
       <c r="AM6" t="b">
         <v>0</v>
       </c>
-      <c r="AN6">
+      <c r="AO6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP6">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -2609,53 +2664,59 @@
       <c r="C7">
         <v>41</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12" t="b">
+      <c r="D7" s="21">
+        <v>0.39019999999999999</v>
+      </c>
+      <c r="E7" s="21">
         <v>1</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="X7" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y7" t="b">
-        <v>1</v>
+      <c r="G7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11" t="b">
+        <v>0</v>
       </c>
       <c r="Z7" t="b">
         <v>0</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AA7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC7" t="s">
         <v>74</v>
       </c>
-      <c r="AB7">
+      <c r="AD7">
         <v>500</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AE7" t="s">
         <v>65</v>
       </c>
-      <c r="AD7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE7">
-        <v>1</v>
-      </c>
-      <c r="AM7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN7">
+      <c r="AF7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG7">
+        <v>1</v>
+      </c>
+      <c r="AO7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP7">
         <v>6.54</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -2665,53 +2726,59 @@
       <c r="C8">
         <v>40</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="12" t="b">
-        <v>1</v>
+      <c r="D8" s="21">
+        <v>0.45</v>
+      </c>
+      <c r="E8" s="21">
+        <v>0.97499999999999998</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="X8" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y8" t="b">
-        <v>1</v>
+      <c r="G8" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11" t="b">
+        <v>0</v>
       </c>
       <c r="Z8" t="b">
         <v>0</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AA8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC8" t="s">
         <v>74</v>
       </c>
-      <c r="AB8">
+      <c r="AD8">
         <v>2000</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AE8" t="s">
         <v>65</v>
       </c>
-      <c r="AD8" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE8">
-        <v>1</v>
-      </c>
-      <c r="AM8" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN8">
+      <c r="AF8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG8">
+        <v>1</v>
+      </c>
+      <c r="AO8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP8">
         <v>9.91</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2721,62 +2788,68 @@
       <c r="C9">
         <v>272</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="b">
-        <v>1</v>
+      <c r="D9" s="22">
+        <v>0.52470000000000006</v>
+      </c>
+      <c r="E9" s="22">
+        <v>0.95440000000000003</v>
       </c>
       <c r="F9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9">
         <v>175</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>55</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>74</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>2000</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>65</v>
       </c>
-      <c r="Q9" t="b">
-        <v>1</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-      <c r="X9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y9" t="b">
-        <v>0</v>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
       </c>
       <c r="Z9" t="b">
         <v>1</v>
       </c>
-      <c r="AM9" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN9">
+      <c r="AA9" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP9">
         <v>26.3</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2786,47 +2859,53 @@
       <c r="C10">
         <v>273</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" t="b">
-        <v>1</v>
+      <c r="D10" s="22">
+        <v>0.44569999999999999</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.93020000000000003</v>
       </c>
       <c r="F10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
       </c>
       <c r="H10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10">
         <v>175</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>55</v>
       </c>
-      <c r="X10" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y10" t="b">
-        <v>0</v>
-      </c>
       <c r="Z10" t="b">
         <v>1</v>
       </c>
-      <c r="AM10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN10">
+      <c r="AA10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO10" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP10">
         <v>26.3</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -2836,63 +2915,67 @@
       <c r="C11">
         <v>46</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="12" t="b">
-        <v>1</v>
+      <c r="D11" s="21">
+        <v>0</v>
+      </c>
+      <c r="E11" s="21">
+        <v>0</v>
       </c>
       <c r="F11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="12" t="b">
-        <v>1</v>
+      <c r="H11" t="b">
+        <v>0</v>
       </c>
       <c r="I11" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="12">
         <v>150</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="M11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12" t="s">
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="O11" s="12">
+      <c r="Q11" s="12">
         <v>500</v>
       </c>
-      <c r="P11" s="12" t="s">
+      <c r="R11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="Q11" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="R11" s="12">
-        <v>1</v>
-      </c>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
+      <c r="S11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" s="12">
+        <v>1</v>
+      </c>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
-      <c r="X11" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="12"/>
-      <c r="AB11" s="12"/>
+      <c r="X11" s="12"/>
+      <c r="Y11" s="12"/>
+      <c r="Z11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB11" t="b">
+        <v>0</v>
+      </c>
       <c r="AC11" s="12"/>
       <c r="AD11" s="12"/>
       <c r="AE11" s="12"/>
@@ -2903,12 +2986,14 @@
       <c r="AJ11" s="12"/>
       <c r="AK11" s="12"/>
       <c r="AL11" s="12"/>
-      <c r="AM11" t="b">
-        <v>1</v>
-      </c>
+      <c r="AM11" s="12"/>
       <c r="AN11" s="12"/>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP11" s="12"/>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -2918,62 +3003,68 @@
       <c r="C12">
         <v>48</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="12" t="b">
-        <v>1</v>
+      <c r="D12" s="21">
+        <v>0</v>
+      </c>
+      <c r="E12" s="21">
+        <v>0.25929999999999997</v>
       </c>
       <c r="F12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="12" t="b">
         <v>1</v>
       </c>
       <c r="H12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12">
         <v>150</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>55</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>74</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>20000</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>65</v>
       </c>
-      <c r="Q12" t="b">
-        <v>1</v>
-      </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-      <c r="X12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y12" t="b">
-        <v>0</v>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
       </c>
       <c r="Z12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN12">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO12" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP12">
         <v>19.7</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2983,11 +3074,11 @@
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" t="b">
-        <v>0</v>
+      <c r="D13" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="21">
+        <v>1</v>
       </c>
       <c r="F13" t="b">
         <v>0</v>
@@ -2998,47 +3089,53 @@
       <c r="H13" t="b">
         <v>0</v>
       </c>
-      <c r="X13" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y13" t="b">
-        <v>1</v>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
       </c>
       <c r="Z13" t="b">
         <v>0</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC13" t="s">
         <v>86</v>
       </c>
-      <c r="AB13">
+      <c r="AD13">
         <v>60</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AE13" t="s">
         <v>65</v>
       </c>
-      <c r="AD13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH13" t="s">
+      <c r="AF13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="s">
         <v>52</v>
       </c>
-      <c r="AI13">
+      <c r="AK13">
         <v>10</v>
       </c>
-      <c r="AJ13" t="s">
+      <c r="AL13" t="s">
         <v>53</v>
       </c>
-      <c r="AK13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL13">
-        <v>1</v>
-      </c>
       <c r="AM13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AN13">
+        <v>1</v>
+      </c>
+      <c r="AO13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3048,11 +3145,11 @@
       <c r="C14">
         <v>6</v>
       </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
+      <c r="D14" s="21">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E14" s="21">
+        <v>1</v>
       </c>
       <c r="F14" t="b">
         <v>0</v>
@@ -3063,47 +3160,53 @@
       <c r="H14" t="b">
         <v>0</v>
       </c>
-      <c r="X14" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="b">
-        <v>1</v>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
       </c>
       <c r="Z14" t="b">
         <v>0</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="AA14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="s">
         <v>86</v>
       </c>
-      <c r="AB14">
+      <c r="AD14">
         <v>80</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AE14" t="s">
         <v>65</v>
       </c>
-      <c r="AD14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH14" t="s">
+      <c r="AF14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="s">
         <v>52</v>
       </c>
-      <c r="AI14">
+      <c r="AK14">
         <v>10</v>
       </c>
-      <c r="AJ14" t="s">
+      <c r="AL14" t="s">
         <v>53</v>
       </c>
-      <c r="AK14" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL14">
-        <v>1</v>
-      </c>
       <c r="AM14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AN14">
+        <v>1</v>
+      </c>
+      <c r="AO14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -3113,11 +3216,11 @@
       <c r="C15">
         <v>76</v>
       </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
+      <c r="D15" s="21">
+        <v>0.3553</v>
+      </c>
+      <c r="E15" s="21">
+        <v>0.98680000000000001</v>
       </c>
       <c r="F15" t="b">
         <v>0</v>
@@ -3128,47 +3231,53 @@
       <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="X15" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y15" t="b">
-        <v>1</v>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
       </c>
       <c r="Z15" t="b">
         <v>0</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AA15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="s">
         <v>86</v>
       </c>
-      <c r="AB15">
+      <c r="AD15">
         <v>60</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AE15" t="s">
         <v>65</v>
       </c>
-      <c r="AD15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH15" t="s">
+      <c r="AF15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="s">
         <v>52</v>
       </c>
-      <c r="AI15">
+      <c r="AK15">
         <v>10</v>
       </c>
-      <c r="AJ15" t="s">
+      <c r="AL15" t="s">
         <v>53</v>
       </c>
-      <c r="AK15" t="b">
-        <v>1</v>
-      </c>
       <c r="AM15" t="b">
         <v>1</v>
       </c>
-      <c r="AN15">
+      <c r="AO15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP15">
         <v>10.8</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -3178,62 +3287,68 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" t="b">
+      <c r="D16" s="22">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="E16" s="22">
         <v>1</v>
       </c>
       <c r="F16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" t="b">
         <v>1</v>
       </c>
       <c r="H16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
       </c>
-      <c r="J16">
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16">
         <v>150</v>
-      </c>
-      <c r="K16" t="s">
-        <v>55</v>
-      </c>
-      <c r="L16">
-        <v>200</v>
       </c>
       <c r="M16" t="s">
         <v>55</v>
       </c>
-      <c r="N16" t="s">
+      <c r="N16">
+        <v>200</v>
+      </c>
+      <c r="O16" t="s">
+        <v>55</v>
+      </c>
+      <c r="P16" t="s">
         <v>96</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>100</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>65</v>
       </c>
-      <c r="Q16" t="b">
-        <v>0</v>
-      </c>
-      <c r="X16" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y16" t="b">
+      <c r="S16" t="b">
         <v>0</v>
       </c>
       <c r="Z16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -3243,62 +3358,68 @@
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" t="b">
+      <c r="D17" s="22">
+        <v>0</v>
+      </c>
+      <c r="E17" s="22">
         <v>1</v>
       </c>
       <c r="F17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="b">
         <v>1</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="J17">
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17">
         <v>150</v>
-      </c>
-      <c r="K17" t="s">
-        <v>55</v>
-      </c>
-      <c r="L17">
-        <v>200</v>
       </c>
       <c r="M17" t="s">
         <v>55</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N17">
+        <v>200</v>
+      </c>
+      <c r="O17" t="s">
+        <v>55</v>
+      </c>
+      <c r="P17" t="s">
         <v>96</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>100</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>65</v>
       </c>
-      <c r="Q17" t="b">
-        <v>0</v>
-      </c>
-      <c r="X17" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y17" t="b">
+      <c r="S17" t="b">
         <v>0</v>
       </c>
       <c r="Z17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB17" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -3308,62 +3429,68 @@
       <c r="C18">
         <v>7</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" t="b">
+      <c r="D18" s="22">
+        <v>0</v>
+      </c>
+      <c r="E18" s="22">
         <v>1</v>
       </c>
       <c r="F18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
         <v>1</v>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
       </c>
-      <c r="J18">
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18">
         <v>150</v>
-      </c>
-      <c r="K18" t="s">
-        <v>55</v>
-      </c>
-      <c r="L18">
-        <v>200</v>
       </c>
       <c r="M18" t="s">
         <v>55</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18">
+        <v>200</v>
+      </c>
+      <c r="O18" t="s">
+        <v>55</v>
+      </c>
+      <c r="P18" t="s">
         <v>96</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>150</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>65</v>
       </c>
-      <c r="Q18" t="b">
-        <v>0</v>
-      </c>
-      <c r="X18" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y18" t="b">
+      <c r="S18" t="b">
         <v>0</v>
       </c>
       <c r="Z18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -3373,65 +3500,71 @@
       <c r="C19">
         <v>138</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" t="b">
+      <c r="D19" s="22">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="E19" s="22">
         <v>1</v>
       </c>
       <c r="F19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" t="b">
         <v>1</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
       </c>
-      <c r="J19">
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19">
         <v>150</v>
-      </c>
-      <c r="K19" t="s">
-        <v>55</v>
-      </c>
-      <c r="L19">
-        <v>200</v>
       </c>
       <c r="M19" t="s">
         <v>55</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19">
+        <v>200</v>
+      </c>
+      <c r="O19" t="s">
+        <v>55</v>
+      </c>
+      <c r="P19" t="s">
         <v>96</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>150</v>
       </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>65</v>
       </c>
-      <c r="Q19" t="b">
-        <v>0</v>
-      </c>
-      <c r="X19" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y19" t="b">
+      <c r="S19" t="b">
         <v>0</v>
       </c>
       <c r="Z19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN19">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP19">
         <v>15.6</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -3441,65 +3574,71 @@
       <c r="C20">
         <v>66</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
+      <c r="D20" s="22">
+        <v>0.36509999999999998</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0.98409999999999997</v>
       </c>
       <c r="F20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" t="b">
         <v>1</v>
       </c>
       <c r="H20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
-      <c r="J20">
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20">
         <v>150</v>
-      </c>
-      <c r="K20" t="s">
-        <v>55</v>
-      </c>
-      <c r="L20">
-        <v>200</v>
       </c>
       <c r="M20" t="s">
         <v>55</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N20">
+        <v>200</v>
+      </c>
+      <c r="O20" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20" t="s">
         <v>101</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>150</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>65</v>
       </c>
-      <c r="Q20" t="b">
-        <v>0</v>
-      </c>
-      <c r="X20" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y20" t="b">
+      <c r="S20" t="b">
         <v>0</v>
       </c>
       <c r="Z20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN20">
+        <v>1</v>
+      </c>
+      <c r="AA20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP20">
         <v>19.3</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -3509,38 +3648,44 @@
       <c r="C21">
         <v>10</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" t="b">
-        <v>0</v>
+      <c r="D21" s="22">
+        <v>0.42859999999999998</v>
+      </c>
+      <c r="E21" s="22">
+        <v>1</v>
       </c>
       <c r="F21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="X21" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y21" t="b">
-        <v>0</v>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
       </c>
       <c r="Z21" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB21" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -3550,38 +3695,44 @@
       <c r="C22">
         <v>7</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" t="b">
-        <v>0</v>
+      <c r="D22" s="22">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="E22" s="22">
+        <v>1</v>
       </c>
       <c r="F22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
       </c>
-      <c r="X22" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y22" t="b">
-        <v>0</v>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
       </c>
       <c r="Z22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB22" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -3591,41 +3742,47 @@
       <c r="C23">
         <v>94</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
+      <c r="D23" s="22">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="E23" s="22">
+        <v>1</v>
       </c>
       <c r="F23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
-      <c r="X23" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y23" t="b">
-        <v>0</v>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
       </c>
       <c r="Z23" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM23" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN23">
+        <v>1</v>
+      </c>
+      <c r="AA23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO23" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP23">
         <v>15.6</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
@@ -3635,11 +3792,11 @@
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" t="b">
-        <v>0</v>
+      <c r="D24" s="23">
+        <v>0.59260000000000002</v>
+      </c>
+      <c r="E24" s="23">
+        <v>0.98870000000000002</v>
       </c>
       <c r="F24" t="b">
         <v>0</v>
@@ -3650,50 +3807,56 @@
       <c r="H24" t="b">
         <v>0</v>
       </c>
-      <c r="X24" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y24" t="b">
-        <v>1</v>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>0</v>
       </c>
       <c r="Z24" t="b">
         <v>0</v>
       </c>
-      <c r="AA24" t="s">
+      <c r="AA24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="s">
         <v>52</v>
       </c>
-      <c r="AB24">
+      <c r="AD24">
         <v>10</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="AE24" t="s">
         <v>53</v>
       </c>
-      <c r="AD24" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE24">
-        <v>1</v>
-      </c>
-      <c r="AH24" t="s">
+      <c r="AF24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG24">
+        <v>1</v>
+      </c>
+      <c r="AJ24" t="s">
         <v>62</v>
       </c>
-      <c r="AI24">
+      <c r="AK24">
         <v>50</v>
       </c>
-      <c r="AJ24" t="s">
+      <c r="AL24" t="s">
         <v>55</v>
       </c>
-      <c r="AK24" t="b">
-        <v>0</v>
-      </c>
       <c r="AM24" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN24">
+        <v>0</v>
+      </c>
+      <c r="AO24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP24">
         <v>12.6</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -3703,11 +3866,11 @@
       <c r="C25">
         <v>13</v>
       </c>
-      <c r="D25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
+      <c r="D25" s="24">
+        <v>0.15379999999999999</v>
+      </c>
+      <c r="E25" s="24">
+        <v>0.84619999999999995</v>
       </c>
       <c r="F25" t="b">
         <v>0</v>
@@ -3718,50 +3881,56 @@
       <c r="H25" t="b">
         <v>0</v>
       </c>
-      <c r="X25" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y25" t="b">
-        <v>1</v>
+      <c r="I25" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
       </c>
       <c r="Z25" t="b">
         <v>0</v>
       </c>
-      <c r="AA25" t="s">
+      <c r="AA25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC25" t="s">
         <v>52</v>
       </c>
-      <c r="AB25">
+      <c r="AD25">
         <v>10</v>
       </c>
-      <c r="AC25" t="s">
+      <c r="AE25" t="s">
         <v>53</v>
       </c>
-      <c r="AD25" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE25">
-        <v>1</v>
-      </c>
-      <c r="AH25" t="s">
+      <c r="AF25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG25">
+        <v>1</v>
+      </c>
+      <c r="AJ25" t="s">
         <v>111</v>
       </c>
-      <c r="AI25">
+      <c r="AK25">
         <v>50</v>
       </c>
-      <c r="AJ25" t="s">
+      <c r="AL25" t="s">
         <v>55</v>
       </c>
-      <c r="AK25" t="b">
-        <v>0</v>
-      </c>
       <c r="AM25" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN25">
+        <v>0</v>
+      </c>
+      <c r="AO25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP25">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -3771,38 +3940,44 @@
       <c r="C26">
         <v>42</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="b">
-        <v>1</v>
+      <c r="D26" s="22">
+        <v>0.31709999999999999</v>
+      </c>
+      <c r="E26" s="22">
+        <v>0.97560000000000002</v>
       </c>
       <c r="F26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" t="b">
         <v>1</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
       </c>
-      <c r="X26" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y26" t="b">
-        <v>0</v>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
       </c>
       <c r="Z26" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB26" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -3812,44 +3987,50 @@
       <c r="C27">
         <v>21</v>
       </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" t="b">
+      <c r="D27" s="22">
+        <v>0.38890000000000002</v>
+      </c>
+      <c r="E27" s="22">
         <v>1</v>
       </c>
       <c r="F27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" t="b">
         <v>1</v>
       </c>
       <c r="H27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
       </c>
-      <c r="J27">
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="L27">
         <v>75</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>55</v>
       </c>
-      <c r="X27" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y27" t="b">
-        <v>0</v>
-      </c>
       <c r="Z27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB27" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8</v>
       </c>
@@ -3859,11 +4040,11 @@
       <c r="C28">
         <v>47</v>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
+      <c r="D28" s="22">
+        <v>0.26190000000000002</v>
+      </c>
+      <c r="E28" s="22">
+        <v>0.57140000000000002</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -3877,35 +4058,41 @@
       <c r="I28" t="b">
         <v>1</v>
       </c>
-      <c r="J28">
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="L28">
         <v>150</v>
-      </c>
-      <c r="K28" t="s">
-        <v>55</v>
-      </c>
-      <c r="L28">
-        <v>200</v>
       </c>
       <c r="M28" t="s">
         <v>55</v>
       </c>
-      <c r="X28" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y28" t="b">
-        <v>0</v>
+      <c r="N28">
+        <v>200</v>
+      </c>
+      <c r="O28" t="s">
+        <v>55</v>
       </c>
       <c r="Z28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN28">
+        <v>1</v>
+      </c>
+      <c r="AA28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP28">
         <v>13.17</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8</v>
       </c>
@@ -3915,11 +4102,11 @@
       <c r="C29">
         <v>52</v>
       </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="b">
-        <v>1</v>
+      <c r="D29" s="22">
+        <v>0.21149999999999999</v>
+      </c>
+      <c r="E29" s="22">
+        <v>0.42309999999999998</v>
       </c>
       <c r="F29" t="b">
         <v>1</v>
@@ -3933,35 +4120,41 @@
       <c r="I29" t="b">
         <v>1</v>
       </c>
-      <c r="J29">
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+      <c r="L29">
         <v>150</v>
-      </c>
-      <c r="K29" t="s">
-        <v>55</v>
-      </c>
-      <c r="L29">
-        <v>200</v>
       </c>
       <c r="M29" t="s">
         <v>55</v>
       </c>
-      <c r="X29" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y29" t="b">
-        <v>0</v>
+      <c r="N29">
+        <v>200</v>
+      </c>
+      <c r="O29" t="s">
+        <v>55</v>
       </c>
       <c r="Z29" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM29" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN29">
+        <v>1</v>
+      </c>
+      <c r="AA29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP29">
         <v>17.579999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14</v>
       </c>
@@ -3971,59 +4164,65 @@
       <c r="C30">
         <v>120</v>
       </c>
-      <c r="D30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" t="b">
-        <v>1</v>
+      <c r="D30" s="21">
+        <v>0.54239999999999999</v>
+      </c>
+      <c r="E30" s="21">
+        <v>0.88139999999999996</v>
       </c>
       <c r="F30" t="b">
         <v>0</v>
       </c>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" t="b">
         <v>0</v>
       </c>
-      <c r="X30" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y30" t="b">
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
         <v>0</v>
       </c>
       <c r="Z30" t="b">
         <v>0</v>
       </c>
-      <c r="AA30" t="s">
+      <c r="AA30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC30" t="s">
         <v>124</v>
       </c>
-      <c r="AB30">
+      <c r="AD30">
         <v>600</v>
       </c>
-      <c r="AC30" t="s">
+      <c r="AE30" t="s">
         <v>65</v>
       </c>
-      <c r="AD30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH30" t="s">
+      <c r="AF30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ30" t="s">
         <v>125</v>
       </c>
-      <c r="AI30">
+      <c r="AK30">
         <v>1000</v>
       </c>
-      <c r="AJ30" t="s">
+      <c r="AL30" t="s">
         <v>65</v>
       </c>
-      <c r="AK30" t="b">
-        <v>0</v>
-      </c>
       <c r="AM30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>14</v>
       </c>
@@ -4033,47 +4232,53 @@
       <c r="C31">
         <v>120</v>
       </c>
-      <c r="D31" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
+      <c r="D31" s="21">
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="E31" s="21">
+        <v>0.67800000000000005</v>
       </c>
       <c r="F31" t="b">
         <v>0</v>
       </c>
       <c r="G31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" t="b">
         <v>0</v>
       </c>
-      <c r="X31" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y31" t="b">
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
         <v>0</v>
       </c>
       <c r="Z31" t="b">
         <v>0</v>
       </c>
-      <c r="AA31" t="s">
+      <c r="AA31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC31" t="s">
         <v>125</v>
       </c>
-      <c r="AB31">
+      <c r="AD31">
         <v>1500</v>
       </c>
-      <c r="AC31" t="s">
+      <c r="AE31" t="s">
         <v>65</v>
       </c>
-      <c r="AD31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AF31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -4083,62 +4288,68 @@
       <c r="C32">
         <v>317</v>
       </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" s="11" t="b">
-        <v>1</v>
+      <c r="D32" s="22">
+        <v>0.38329999999999997</v>
+      </c>
+      <c r="E32" s="22">
+        <v>0.97330000000000005</v>
       </c>
       <c r="F32" t="b">
-        <v>0</v>
-      </c>
-      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
       </c>
-      <c r="J32">
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="b">
+        <v>1</v>
+      </c>
+      <c r="L32">
         <v>75</v>
       </c>
-      <c r="K32" t="s">
+      <c r="M32" t="s">
         <v>55</v>
       </c>
-      <c r="N32" t="s">
+      <c r="P32" t="s">
         <v>101</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>10</v>
       </c>
-      <c r="P32" t="s">
+      <c r="R32" t="s">
         <v>53</v>
       </c>
-      <c r="Q32" t="b">
-        <v>1</v>
-      </c>
-      <c r="R32">
-        <v>1</v>
-      </c>
-      <c r="X32" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y32" t="b">
-        <v>0</v>
+      <c r="S32" t="b">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
       </c>
       <c r="Z32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM32" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN32">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP32">
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -4148,62 +4359,68 @@
       <c r="C33">
         <v>320</v>
       </c>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="11" t="b">
-        <v>1</v>
+      <c r="D33" s="22">
+        <v>0.46529999999999999</v>
+      </c>
+      <c r="E33" s="22">
+        <v>0.96730000000000005</v>
       </c>
       <c r="F33" t="b">
-        <v>0</v>
-      </c>
-      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="11" t="b">
         <v>1</v>
       </c>
       <c r="H33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
-      <c r="J33">
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
+      <c r="L33">
         <v>75</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" t="s">
         <v>55</v>
       </c>
-      <c r="N33" t="s">
+      <c r="P33" t="s">
         <v>52</v>
       </c>
-      <c r="O33">
+      <c r="Q33">
         <v>10</v>
       </c>
-      <c r="P33" t="s">
+      <c r="R33" t="s">
         <v>53</v>
       </c>
-      <c r="Q33" t="b">
-        <v>1</v>
-      </c>
-      <c r="R33">
-        <v>1</v>
-      </c>
-      <c r="X33" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y33" t="b">
-        <v>0</v>
+      <c r="S33" t="b">
+        <v>1</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
       </c>
       <c r="Z33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM33" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN33">
+        <v>1</v>
+      </c>
+      <c r="AA33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO33" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP33">
         <v>15.7</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15</v>
       </c>
@@ -4213,71 +4430,77 @@
       <c r="C34">
         <v>29</v>
       </c>
-      <c r="D34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
+      <c r="D34" s="21">
+        <v>0.24</v>
+      </c>
+      <c r="E34" s="21">
+        <v>0.8</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
       </c>
       <c r="G34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
       </c>
-      <c r="X34" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y34" t="b">
-        <v>1</v>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>0</v>
       </c>
       <c r="Z34" t="b">
         <v>0</v>
       </c>
-      <c r="AA34" t="s">
+      <c r="AA34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="s">
         <v>138</v>
       </c>
-      <c r="AB34">
+      <c r="AD34">
         <v>0.4</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AE34" t="s">
         <v>139</v>
       </c>
-      <c r="AD34" t="b">
-        <v>0</v>
-      </c>
       <c r="AF34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG34">
+        <v>0</v>
+      </c>
+      <c r="AH34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI34">
         <v>0.5</v>
       </c>
-      <c r="AH34" t="s">
+      <c r="AJ34" t="s">
         <v>52</v>
       </c>
-      <c r="AI34">
+      <c r="AK34">
         <v>10</v>
       </c>
-      <c r="AJ34" t="s">
+      <c r="AL34" t="s">
         <v>53</v>
       </c>
-      <c r="AK34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL34">
-        <v>1</v>
-      </c>
       <c r="AM34" t="b">
         <v>1</v>
       </c>
       <c r="AN34">
+        <v>1</v>
+      </c>
+      <c r="AO34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP34">
         <v>6.6</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15</v>
       </c>
@@ -4287,71 +4510,77 @@
       <c r="C35">
         <v>30</v>
       </c>
-      <c r="D35" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
+      <c r="D35" s="21">
+        <v>0.35709999999999997</v>
+      </c>
+      <c r="E35" s="21">
+        <v>0.82140000000000002</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
       </c>
       <c r="G35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
       </c>
-      <c r="X35" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y35" t="b">
-        <v>1</v>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
       </c>
       <c r="Z35" t="b">
         <v>0</v>
       </c>
-      <c r="AA35" t="s">
+      <c r="AA35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC35" t="s">
         <v>138</v>
       </c>
-      <c r="AB35">
+      <c r="AD35">
         <v>0.4</v>
       </c>
-      <c r="AC35" t="s">
+      <c r="AE35" t="s">
         <v>139</v>
       </c>
-      <c r="AD35" t="b">
-        <v>0</v>
-      </c>
       <c r="AF35" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG35">
+        <v>0</v>
+      </c>
+      <c r="AH35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI35">
         <v>0.5</v>
       </c>
-      <c r="AH35" t="s">
+      <c r="AJ35" t="s">
         <v>52</v>
       </c>
-      <c r="AI35">
+      <c r="AK35">
         <v>10</v>
       </c>
-      <c r="AJ35" t="s">
+      <c r="AL35" t="s">
         <v>53</v>
       </c>
-      <c r="AK35" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL35">
-        <v>1</v>
-      </c>
       <c r="AM35" t="b">
         <v>1</v>
       </c>
       <c r="AN35">
+        <v>1</v>
+      </c>
+      <c r="AO35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP35">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -4361,53 +4590,59 @@
       <c r="C36">
         <v>31</v>
       </c>
-      <c r="D36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
+      <c r="D36" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="E36" s="22">
+        <v>0.9</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
       </c>
       <c r="G36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36" t="b">
         <v>0</v>
       </c>
-      <c r="X36" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y36" t="b">
-        <v>1</v>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>0</v>
       </c>
       <c r="Z36" t="b">
         <v>0</v>
       </c>
-      <c r="AA36" t="s">
+      <c r="AA36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB36" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC36" t="s">
         <v>52</v>
       </c>
-      <c r="AB36">
+      <c r="AD36">
         <v>10</v>
       </c>
-      <c r="AC36" t="s">
+      <c r="AE36" t="s">
         <v>53</v>
       </c>
-      <c r="AD36" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE36">
-        <v>1</v>
-      </c>
-      <c r="AM36" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN36">
+      <c r="AF36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG36">
+        <v>1</v>
+      </c>
+      <c r="AO36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AP36">
         <v>10.7</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16</v>
       </c>
@@ -4417,59 +4652,65 @@
       <c r="C37">
         <v>8</v>
       </c>
-      <c r="D37" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
+      <c r="D37" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="E37" s="22">
+        <v>0.875</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
       </c>
       <c r="G37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" t="b">
         <v>0</v>
       </c>
-      <c r="X37" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y37" t="b">
-        <v>1</v>
+      <c r="I37" t="b">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
       </c>
       <c r="Z37" t="b">
         <v>0</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="AA37" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC37" t="s">
         <v>144</v>
       </c>
-      <c r="AB37">
+      <c r="AD37">
         <v>20</v>
       </c>
-      <c r="AC37" t="s">
+      <c r="AE37" t="s">
         <v>65</v>
       </c>
-      <c r="AD37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH37" t="s">
+      <c r="AF37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ37" t="s">
         <v>62</v>
       </c>
-      <c r="AI37">
+      <c r="AK37">
         <v>60</v>
       </c>
-      <c r="AJ37" t="s">
+      <c r="AL37" t="s">
         <v>65</v>
       </c>
-      <c r="AK37" t="b">
-        <v>0</v>
-      </c>
       <c r="AM37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
@@ -4479,59 +4720,65 @@
       <c r="C38">
         <v>7</v>
       </c>
-      <c r="D38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
+      <c r="D38" s="21">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E38" s="21">
+        <v>0.83330000000000004</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
       </c>
       <c r="G38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38" t="b">
         <v>0</v>
       </c>
-      <c r="X38" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y38" t="b">
-        <v>1</v>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <v>0</v>
       </c>
       <c r="Z38" t="b">
         <v>0</v>
       </c>
-      <c r="AA38" t="s">
+      <c r="AA38" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC38" t="s">
         <v>144</v>
       </c>
-      <c r="AB38">
+      <c r="AD38">
         <v>40</v>
       </c>
-      <c r="AC38" t="s">
+      <c r="AE38" t="s">
         <v>65</v>
       </c>
-      <c r="AD38" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH38" t="s">
+      <c r="AF38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ38" t="s">
         <v>62</v>
       </c>
-      <c r="AI38">
+      <c r="AK38">
         <v>60</v>
       </c>
-      <c r="AJ38" t="s">
+      <c r="AL38" t="s">
         <v>65</v>
       </c>
-      <c r="AK38" t="b">
-        <v>0</v>
-      </c>
       <c r="AM38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>16</v>
       </c>
@@ -4541,59 +4788,65 @@
       <c r="C39">
         <v>8</v>
       </c>
-      <c r="D39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
+      <c r="D39" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="E39" s="21">
+        <v>0.75</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
       </c>
       <c r="G39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" t="b">
         <v>0</v>
       </c>
-      <c r="X39" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y39" t="b">
-        <v>1</v>
+      <c r="I39" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" t="b">
+        <v>0</v>
       </c>
       <c r="Z39" t="b">
         <v>0</v>
       </c>
-      <c r="AA39" t="s">
+      <c r="AA39" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC39" t="s">
         <v>144</v>
       </c>
-      <c r="AB39">
+      <c r="AD39">
         <v>40</v>
       </c>
-      <c r="AC39" t="s">
+      <c r="AE39" t="s">
         <v>65</v>
       </c>
-      <c r="AD39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH39" t="s">
+      <c r="AF39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ39" t="s">
         <v>62</v>
       </c>
-      <c r="AI39">
+      <c r="AK39">
         <v>75</v>
       </c>
-      <c r="AJ39" t="s">
+      <c r="AL39" t="s">
         <v>65</v>
       </c>
-      <c r="AK39" t="b">
-        <v>0</v>
-      </c>
       <c r="AM39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>16</v>
       </c>
@@ -4603,62 +4856,68 @@
       <c r="C40">
         <v>75</v>
       </c>
-      <c r="D40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
+      <c r="D40" s="21">
+        <v>0.26029999999999998</v>
+      </c>
+      <c r="E40" s="21">
+        <v>0.95889999999999997</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
       </c>
       <c r="G40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40" t="b">
         <v>0</v>
       </c>
-      <c r="X40" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y40" t="b">
-        <v>1</v>
+      <c r="I40" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" t="b">
+        <v>0</v>
       </c>
       <c r="Z40" t="b">
         <v>0</v>
       </c>
-      <c r="AA40" t="s">
+      <c r="AA40" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC40" t="s">
         <v>144</v>
       </c>
-      <c r="AB40">
+      <c r="AD40">
         <v>40</v>
       </c>
-      <c r="AC40" t="s">
+      <c r="AE40" t="s">
         <v>65</v>
       </c>
-      <c r="AD40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH40" t="s">
+      <c r="AF40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ40" t="s">
         <v>62</v>
       </c>
-      <c r="AI40">
+      <c r="AK40">
         <v>75</v>
       </c>
-      <c r="AJ40" t="s">
+      <c r="AL40" t="s">
         <v>65</v>
       </c>
-      <c r="AK40" t="b">
-        <v>0</v>
-      </c>
       <c r="AM40" t="b">
         <v>0</v>
       </c>
-      <c r="AN40">
+      <c r="AO40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP40">
         <v>10.3</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>16</v>
       </c>
@@ -4668,62 +4927,68 @@
       <c r="C41">
         <v>76</v>
       </c>
-      <c r="D41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" t="b">
-        <v>1</v>
+      <c r="D41" s="21">
+        <v>0.20549999999999999</v>
+      </c>
+      <c r="E41" s="21">
+        <v>0.95889999999999997</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
       </c>
       <c r="G41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" t="b">
         <v>0</v>
       </c>
-      <c r="X41" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y41" t="b">
-        <v>1</v>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <v>0</v>
       </c>
       <c r="Z41" t="b">
         <v>0</v>
       </c>
-      <c r="AA41" t="s">
+      <c r="AA41" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC41" t="s">
         <v>144</v>
       </c>
-      <c r="AB41">
+      <c r="AD41">
         <v>40</v>
       </c>
-      <c r="AC41" t="s">
+      <c r="AE41" t="s">
         <v>65</v>
       </c>
-      <c r="AD41" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH41" t="s">
+      <c r="AF41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ41" t="s">
         <v>62</v>
       </c>
-      <c r="AI41">
+      <c r="AK41">
         <v>150</v>
       </c>
-      <c r="AJ41" t="s">
+      <c r="AL41" t="s">
         <v>65</v>
       </c>
-      <c r="AK41" t="b">
-        <v>0</v>
-      </c>
       <c r="AM41" t="b">
         <v>0</v>
       </c>
-      <c r="AN41">
+      <c r="AO41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP41">
         <v>10.7</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>16</v>
       </c>
@@ -4733,62 +4998,68 @@
       <c r="C42">
         <v>36</v>
       </c>
-      <c r="D42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
+      <c r="D42" s="21">
+        <v>0.4375</v>
+      </c>
+      <c r="E42" s="21">
+        <v>0.96879999999999999</v>
       </c>
       <c r="F42" t="b">
         <v>0</v>
       </c>
       <c r="G42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" t="b">
         <v>0</v>
       </c>
-      <c r="X42" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y42" t="b">
-        <v>1</v>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>0</v>
       </c>
       <c r="Z42" t="b">
         <v>0</v>
       </c>
-      <c r="AA42" t="s">
+      <c r="AA42" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC42" t="s">
         <v>144</v>
       </c>
-      <c r="AB42">
+      <c r="AD42">
         <v>40</v>
       </c>
-      <c r="AC42" t="s">
+      <c r="AE42" t="s">
         <v>65</v>
       </c>
-      <c r="AD42" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH42" t="s">
+      <c r="AF42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ42" t="s">
         <v>62</v>
       </c>
-      <c r="AI42">
+      <c r="AK42">
         <v>75</v>
       </c>
-      <c r="AJ42" t="s">
+      <c r="AL42" t="s">
         <v>65</v>
       </c>
-      <c r="AK42" t="b">
-        <v>0</v>
-      </c>
       <c r="AM42" t="b">
         <v>0</v>
       </c>
-      <c r="AN42">
+      <c r="AO42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP42">
         <v>4.7</v>
       </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -4798,56 +5069,62 @@
       <c r="C43">
         <v>12</v>
       </c>
-      <c r="D43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" t="b">
-        <v>0</v>
+      <c r="D43" s="21">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="E43" s="21">
+        <v>1</v>
       </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
-      <c r="J43">
+      <c r="J43" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" t="b">
+        <v>1</v>
+      </c>
+      <c r="L43">
         <v>150</v>
       </c>
-      <c r="K43" t="s">
+      <c r="M43" t="s">
         <v>55</v>
       </c>
-      <c r="N43" t="s">
+      <c r="P43" t="s">
         <v>154</v>
       </c>
-      <c r="O43">
+      <c r="Q43">
         <v>500</v>
       </c>
-      <c r="P43" t="s">
+      <c r="R43" t="s">
         <v>65</v>
       </c>
-      <c r="Q43" t="b">
-        <v>0</v>
-      </c>
-      <c r="X43" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y43" t="b">
+      <c r="S43" t="b">
         <v>0</v>
       </c>
       <c r="Z43" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA43" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB43" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -4857,56 +5134,62 @@
       <c r="C44">
         <v>3</v>
       </c>
-      <c r="D44" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" t="b">
-        <v>0</v>
+      <c r="D44" s="21">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="E44" s="21">
+        <v>1</v>
       </c>
       <c r="F44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="b">
         <v>1</v>
       </c>
-      <c r="J44">
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+      <c r="K44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44">
         <v>150</v>
       </c>
-      <c r="K44" t="s">
+      <c r="M44" t="s">
         <v>55</v>
       </c>
-      <c r="N44" t="s">
+      <c r="P44" t="s">
         <v>154</v>
       </c>
-      <c r="O44">
+      <c r="Q44">
         <v>500</v>
       </c>
-      <c r="P44" t="s">
+      <c r="R44" t="s">
         <v>65</v>
       </c>
-      <c r="Q44" t="b">
-        <v>0</v>
-      </c>
-      <c r="X44" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y44" t="b">
+      <c r="S44" t="b">
         <v>0</v>
       </c>
       <c r="Z44" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA44" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB44" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -4916,56 +5199,62 @@
       <c r="C45">
         <v>110</v>
       </c>
-      <c r="D45" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" t="b">
-        <v>0</v>
+      <c r="D45" s="21">
+        <v>0.58879999999999999</v>
+      </c>
+      <c r="E45" s="21">
+        <v>0.99070000000000003</v>
       </c>
       <c r="F45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
       </c>
-      <c r="J45">
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45">
         <v>150</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M45" t="s">
         <v>55</v>
       </c>
-      <c r="N45" t="s">
+      <c r="P45" t="s">
         <v>154</v>
       </c>
-      <c r="O45">
+      <c r="Q45">
         <v>400</v>
       </c>
-      <c r="P45" t="s">
+      <c r="R45" t="s">
         <v>65</v>
       </c>
-      <c r="Q45" t="b">
-        <v>0</v>
-      </c>
-      <c r="X45" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y45" t="b">
+      <c r="S45" t="b">
         <v>0</v>
       </c>
       <c r="Z45" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="AA45" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB45" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>16</v>
       </c>
@@ -4975,59 +5264,65 @@
       <c r="C46">
         <v>9</v>
       </c>
-      <c r="D46" t="b">
-        <v>0</v>
-      </c>
-      <c r="E46" t="b">
+      <c r="D46" s="21">
+        <v>0.1111</v>
+      </c>
+      <c r="E46" s="21">
         <v>1</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
       </c>
       <c r="G46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
       </c>
-      <c r="X46" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y46" t="b">
-        <v>1</v>
+      <c r="I46" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" t="b">
+        <v>0</v>
       </c>
       <c r="Z46" t="b">
         <v>0</v>
       </c>
-      <c r="AA46" t="s">
+      <c r="AA46" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC46" t="s">
         <v>144</v>
       </c>
-      <c r="AB46">
+      <c r="AD46">
         <v>20</v>
       </c>
-      <c r="AC46" t="s">
+      <c r="AE46" t="s">
         <v>65</v>
       </c>
-      <c r="AD46" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH46" t="s">
+      <c r="AF46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ46" t="s">
         <v>62</v>
       </c>
-      <c r="AI46">
+      <c r="AK46">
         <v>75</v>
       </c>
-      <c r="AJ46" t="s">
+      <c r="AL46" t="s">
         <v>65</v>
       </c>
-      <c r="AK46" t="b">
-        <v>0</v>
-      </c>
       <c r="AM46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AO46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>16</v>
       </c>
@@ -5037,58 +5332,64 @@
       <c r="C47">
         <v>38</v>
       </c>
-      <c r="D47" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" t="b">
-        <v>1</v>
+      <c r="D47" s="21">
+        <v>0.27029999999999998</v>
+      </c>
+      <c r="E47" s="21">
+        <v>0.8649</v>
       </c>
       <c r="F47" t="b">
         <v>0</v>
       </c>
       <c r="G47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47" t="b">
         <v>0</v>
       </c>
-      <c r="X47" t="b">
-        <v>0</v>
-      </c>
-      <c r="Y47" t="b">
-        <v>1</v>
+      <c r="I47" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" t="b">
+        <v>0</v>
       </c>
       <c r="Z47" t="b">
         <v>0</v>
       </c>
-      <c r="AA47" t="s">
+      <c r="AA47" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC47" t="s">
         <v>144</v>
       </c>
-      <c r="AB47">
+      <c r="AD47">
         <v>40</v>
       </c>
-      <c r="AC47" t="s">
+      <c r="AE47" t="s">
         <v>65</v>
       </c>
-      <c r="AD47" t="b">
-        <v>0</v>
-      </c>
-      <c r="AH47" t="s">
+      <c r="AF47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ47" t="s">
         <v>62</v>
       </c>
-      <c r="AI47">
+      <c r="AK47">
         <v>150</v>
       </c>
-      <c r="AJ47" t="s">
+      <c r="AL47" t="s">
         <v>65</v>
       </c>
-      <c r="AK47" t="b">
-        <v>0</v>
-      </c>
       <c r="AM47" t="b">
         <v>0</v>
       </c>
-      <c r="AN47">
+      <c r="AO47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP47">
         <v>4.7</v>
       </c>
     </row>
@@ -5104,7 +5405,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
+    <sheetView topLeftCell="A119" workbookViewId="0">
       <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Emily's 'Burden' Comparison
</commit_message>
<xml_diff>
--- a/variable-dosing_7119.xlsx
+++ b/variable-dosing_7119.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaston\Desktop\GBM-master\GBM-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{309D8BCE-5128-42A5-B14C-08A41333CAC8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7807F286-5440-433B-B123-5492AA6CC685}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Concomitant" sheetId="6" r:id="rId5"/>
     <sheet name="Concomitant Tem" sheetId="7" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="698" uniqueCount="170">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="729" uniqueCount="171">
   <si>
     <t>Phase</t>
   </si>
@@ -546,6 +549,9 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>BurdenTwo</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1182,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1220,6 +1226,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1504,6 +1511,29 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Studies"/>
+      <sheetName val="Arms"/>
+      <sheetName val="Dropout"/>
+      <sheetName val="Neoadjuvant"/>
+      <sheetName val="Concomitant"/>
+      <sheetName val="Concomitant Tem"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5BE1F00-7C86-4C71-9EAE-ECCFACB9E11D}" name="Table1" displayName="Table1" ref="A1:C18" totalsRowShown="0">
   <autoFilter ref="A1:C18" xr:uid="{D3BE7780-923D-4844-9487-54D20421F434}"/>
@@ -1517,15 +1547,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2A8E3CB-1AFB-479A-A935-6E3A8A8C1E2A}" name="Table2" displayName="Table2" ref="A1:AQ1048576" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:AQ1048576" xr:uid="{337B527E-CC89-49CB-B8CF-29513C2E5B70}">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="High"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="43">
+<table xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B2A8E3CB-1AFB-479A-A935-6E3A8A8C1E2A}" name="Table2" displayName="Table2" ref="A1:AR1048576" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:AR1048576" xr:uid="{337B527E-CC89-49CB-B8CF-29513C2E5B70}"/>
+  <tableColumns count="44">
     <tableColumn id="1" xr3:uid="{04959165-9B47-46FC-95B1-128303AC6772}" name="NCT"/>
     <tableColumn id="2" xr3:uid="{749B59FF-4A21-40FD-8008-2136ADB4D3D2}" name="Arm"/>
     <tableColumn id="3" xr3:uid="{812D4910-70D1-4BB6-9392-9EE81E6B607E}" name="Enrollment"/>
@@ -1536,6 +1560,7 @@
     <tableColumn id="10" xr3:uid="{03B678CC-1932-4A2C-AAB0-73B5893DD292}" name="Surgery"/>
     <tableColumn id="51" xr3:uid="{41084609-8915-4406-AFEA-4170D289E825}" name="Universal IV"/>
     <tableColumn id="12" xr3:uid="{13578889-6BE7-4CFA-979E-2BB08302CFB7}" name="Burden" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{F0F339F0-4E08-4DB3-8E47-281D3B66A356}" name="BurdenTwo"/>
     <tableColumn id="11" xr3:uid="{FA550D66-7A8A-4FDA-A4AD-2318054511FD}" name="Concomitant"/>
     <tableColumn id="20" xr3:uid="{74EFA571-B2A7-46A2-9E15-B8698BFB18EB}" name="Adjuvant"/>
     <tableColumn id="21" xr3:uid="{B9C7D220-7D77-4400-A952-69BE0E445DC4}" name="Adjuvant TEM"/>
@@ -2144,13 +2169,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AQ47"/>
+  <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="75.75" customWidth="1"/>
     <col min="3" max="3" width="10.25" customWidth="1"/>
@@ -2159,42 +2184,44 @@
     <col min="6" max="6" width="9.875" customWidth="1"/>
     <col min="7" max="7" width="11.125" customWidth="1"/>
     <col min="8" max="8" width="12.75" customWidth="1"/>
-    <col min="9" max="10" width="29.875" customWidth="1"/>
-    <col min="11" max="11" width="13.75" customWidth="1"/>
-    <col min="12" max="12" width="27.75" customWidth="1"/>
-    <col min="13" max="13" width="20.625" customWidth="1"/>
-    <col min="14" max="14" width="13.5" customWidth="1"/>
-    <col min="15" max="15" width="20.75" customWidth="1"/>
-    <col min="16" max="16" width="24.125" customWidth="1"/>
-    <col min="17" max="17" width="20.75" customWidth="1"/>
-    <col min="18" max="18" width="23.375" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
-    <col min="20" max="20" width="20.875" customWidth="1"/>
-    <col min="21" max="21" width="24.75" customWidth="1"/>
-    <col min="22" max="22" width="19.625" customWidth="1"/>
-    <col min="23" max="23" width="28.75" customWidth="1"/>
-    <col min="24" max="24" width="15" customWidth="1"/>
-    <col min="25" max="25" width="20.875" customWidth="1"/>
-    <col min="26" max="26" width="24.75" customWidth="1"/>
-    <col min="27" max="27" width="19.625" customWidth="1"/>
-    <col min="28" max="28" width="28.75" customWidth="1"/>
-    <col min="31" max="31" width="11.875" customWidth="1"/>
-    <col min="32" max="32" width="16.125" customWidth="1"/>
-    <col min="33" max="33" width="20.375" customWidth="1"/>
-    <col min="34" max="34" width="24.125" customWidth="1"/>
-    <col min="35" max="35" width="20.75" customWidth="1"/>
-    <col min="36" max="36" width="29.875" customWidth="1"/>
-    <col min="37" max="37" width="13.25" customWidth="1"/>
-    <col min="38" max="38" width="22.375" customWidth="1"/>
-    <col min="39" max="39" width="16.125" customWidth="1"/>
-    <col min="40" max="40" width="22.875" customWidth="1"/>
-    <col min="41" max="41" width="28.5" customWidth="1"/>
-    <col min="42" max="42" width="20.375" customWidth="1"/>
-    <col min="44" max="44" width="12.125" customWidth="1"/>
-    <col min="45" max="45" width="22.375" customWidth="1"/>
+    <col min="9" max="9" width="29.875" customWidth="1"/>
+    <col min="10" max="10" width="29.875" style="25" customWidth="1"/>
+    <col min="11" max="11" width="29.875" customWidth="1"/>
+    <col min="12" max="12" width="13.75" customWidth="1"/>
+    <col min="13" max="13" width="27.75" customWidth="1"/>
+    <col min="14" max="14" width="20.625" customWidth="1"/>
+    <col min="15" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="16" width="20.75" customWidth="1"/>
+    <col min="17" max="17" width="24.125" customWidth="1"/>
+    <col min="18" max="18" width="20.75" customWidth="1"/>
+    <col min="19" max="19" width="23.375" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="20.875" customWidth="1"/>
+    <col min="22" max="22" width="24.75" customWidth="1"/>
+    <col min="23" max="23" width="19.625" customWidth="1"/>
+    <col min="24" max="24" width="28.75" customWidth="1"/>
+    <col min="25" max="25" width="15" customWidth="1"/>
+    <col min="26" max="26" width="20.875" customWidth="1"/>
+    <col min="27" max="27" width="24.75" customWidth="1"/>
+    <col min="28" max="28" width="19.625" customWidth="1"/>
+    <col min="29" max="29" width="28.75" customWidth="1"/>
+    <col min="32" max="32" width="11.875" customWidth="1"/>
+    <col min="33" max="33" width="16.125" customWidth="1"/>
+    <col min="34" max="34" width="20.375" customWidth="1"/>
+    <col min="35" max="35" width="24.125" customWidth="1"/>
+    <col min="36" max="36" width="20.75" customWidth="1"/>
+    <col min="37" max="37" width="29.875" customWidth="1"/>
+    <col min="38" max="38" width="13.25" customWidth="1"/>
+    <col min="39" max="39" width="22.375" customWidth="1"/>
+    <col min="40" max="40" width="16.125" customWidth="1"/>
+    <col min="41" max="41" width="22.875" customWidth="1"/>
+    <col min="42" max="42" width="28.5" customWidth="1"/>
+    <col min="43" max="43" width="20.375" customWidth="1"/>
+    <col min="45" max="45" width="12.125" customWidth="1"/>
+    <col min="46" max="46" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>158</v>
       </c>
@@ -2226,106 +2253,109 @@
         <v>166</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="U1" s="9" t="s">
+      <c r="V1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="9" t="s">
+      <c r="W1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="X1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="Y1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Z1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="AA1" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AB1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AF1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AG1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AH1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AL1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AM1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AN1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AO1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AP1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AQ1" s="8" t="s">
+      <c r="AR1" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2353,63 +2383,66 @@
       <c r="I2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" t="str">
+      <c r="J2" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K2" t="b">
-        <v>1</v>
+      <c r="K2" t="s">
+        <v>169</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
       </c>
       <c r="M2" t="b">
-        <v>0</v>
-      </c>
-      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>52</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>10</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>53</v>
       </c>
-      <c r="U2" t="b">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="V2" t="b">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2" t="s">
         <v>54</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>125</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA2">
+      <c r="AA2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB2">
         <v>1.5</v>
       </c>
-      <c r="AB2" t="b">
-        <v>1</v>
-      </c>
       <c r="AC2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD2" t="b">
         <v>0</v>
       </c>
-      <c r="AQ2">
+      <c r="AE2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR2">
         <v>16.64</v>
       </c>
     </row>
-    <row r="3" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2437,11 +2470,11 @@
       <c r="I3" t="b">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="K3" t="b">
-        <v>1</v>
+      <c r="K3" t="s">
+        <v>168</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
@@ -2449,26 +2482,29 @@
       <c r="M3" t="b">
         <v>1</v>
       </c>
-      <c r="N3">
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>175</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>55</v>
       </c>
-      <c r="AB3" t="b">
-        <v>1</v>
-      </c>
       <c r="AC3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3" t="b">
         <v>0</v>
       </c>
-      <c r="AQ3">
+      <c r="AE3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR3">
         <v>17.3</v>
       </c>
     </row>
-    <row r="4" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2496,17 +2532,19 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
-      <c r="J4" t="str">
+      <c r="J4" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K4" s="11" t="b">
-        <v>0</v>
+      <c r="K4" t="s">
+        <v>169</v>
       </c>
       <c r="L4" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="M4" s="11"/>
+      <c r="M4" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
@@ -2521,28 +2559,28 @@
       <c r="Y4" s="11"/>
       <c r="Z4" s="11"/>
       <c r="AA4" s="11"/>
-      <c r="AB4" s="11" t="b">
-        <v>0</v>
-      </c>
+      <c r="AB4" s="11"/>
       <c r="AC4" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AF4" s="11">
+      <c r="AG4" s="11">
         <v>30</v>
       </c>
-      <c r="AG4" s="11" t="s">
+      <c r="AH4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AH4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI4" s="11"/>
+      <c r="AI4" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="AJ4" s="11"/>
       <c r="AK4" s="11"/>
       <c r="AL4" s="11"/>
@@ -2550,11 +2588,12 @@
       <c r="AN4" s="11"/>
       <c r="AO4" s="11"/>
       <c r="AP4" s="11"/>
-      <c r="AQ4" s="11">
+      <c r="AQ4" s="11"/>
+      <c r="AR4" s="11">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -2582,54 +2621,57 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-      <c r="J5" t="str">
+      <c r="J5" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K5" s="11" t="b">
-        <v>0</v>
+      <c r="K5" t="s">
+        <v>169</v>
       </c>
       <c r="L5" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="AB5" s="11" t="b">
+      <c r="M5" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AC5" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>20</v>
       </c>
-      <c r="AG5" s="11" t="s">
+      <c r="AH5" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AH5" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL5" t="s">
+      <c r="AI5" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="s">
         <v>69</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>110</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>55</v>
       </c>
-      <c r="AO5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ5">
+      <c r="AP5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR5">
         <v>9.4</v>
       </c>
     </row>
-    <row r="6" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -2657,54 +2699,57 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
-      <c r="J6" t="str">
+      <c r="J6" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K6" s="11" t="b">
-        <v>0</v>
+      <c r="K6" t="s">
+        <v>169</v>
       </c>
       <c r="L6" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="AB6" s="11" t="b">
+      <c r="M6" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AC6" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="s">
         <v>69</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>110</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>55</v>
       </c>
-      <c r="AH6" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL6" t="s">
+      <c r="AI6" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM6" t="s">
         <v>71</v>
       </c>
-      <c r="AM6">
+      <c r="AN6">
         <v>20</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>65</v>
       </c>
-      <c r="AO6" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
+      <c r="AP6" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR6">
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
@@ -2732,45 +2777,49 @@
       <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="J7" t="str">
+      <c r="J7" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K7" s="11" t="b">
-        <v>0</v>
+      <c r="K7" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L7" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="AB7" t="b">
+      <c r="M7" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AC7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE7" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF7" t="s">
         <v>74</v>
       </c>
-      <c r="AF7">
+      <c r="AG7">
         <v>500</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>65</v>
       </c>
-      <c r="AH7" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI7">
-        <v>1</v>
-      </c>
-      <c r="AQ7">
+      <c r="AI7" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ7">
+        <v>1</v>
+      </c>
+      <c r="AR7">
         <v>6.54</v>
       </c>
     </row>
-    <row r="8" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -2798,45 +2847,48 @@
       <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="J8" t="str">
+      <c r="J8" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K8" s="11" t="b">
-        <v>0</v>
+      <c r="K8" t="s">
+        <v>167</v>
       </c>
       <c r="L8" s="11" t="b">
         <v>0</v>
       </c>
-      <c r="AB8" t="b">
+      <c r="M8" s="11" t="b">
         <v>0</v>
       </c>
       <c r="AC8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF8" t="s">
         <v>74</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>2000</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AH8" t="s">
         <v>65</v>
       </c>
-      <c r="AH8" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI8">
-        <v>1</v>
-      </c>
-      <c r="AQ8">
+      <c r="AI8" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>1</v>
+      </c>
+      <c r="AR8">
         <v>9.91</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -2864,12 +2916,13 @@
       <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="J9" t="str">
+      <c r="J9" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K9" t="b">
-        <v>1</v>
+      <c r="K9" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
@@ -2877,41 +2930,44 @@
       <c r="M9" t="b">
         <v>1</v>
       </c>
-      <c r="N9">
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="O9">
         <v>175</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>55</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>74</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>2000</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>65</v>
       </c>
-      <c r="U9" t="b">
-        <v>1</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="AB9" t="b">
+      <c r="V9" t="b">
+        <v>1</v>
+      </c>
+      <c r="W9">
         <v>1</v>
       </c>
       <c r="AC9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD9" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AE9" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR9">
         <v>26.3</v>
       </c>
     </row>
-    <row r="10" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2939,12 +2995,13 @@
       <c r="I10" t="b">
         <v>0</v>
       </c>
-      <c r="J10" t="str">
+      <c r="J10" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K10" t="b">
-        <v>1</v>
+      <c r="K10" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
@@ -2952,26 +3009,29 @@
       <c r="M10" t="b">
         <v>1</v>
       </c>
-      <c r="N10">
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <v>175</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>55</v>
       </c>
-      <c r="AB10" t="b">
-        <v>1</v>
-      </c>
       <c r="AC10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD10" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ10">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR10">
         <v>26.3</v>
       </c>
     </row>
-    <row r="11" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -2999,12 +3059,12 @@
       <c r="I11" t="b">
         <v>1</v>
       </c>
-      <c r="J11" t="str">
+      <c r="J11" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K11" s="12" t="b">
-        <v>1</v>
+      <c r="K11" t="s">
+        <v>169</v>
       </c>
       <c r="L11" s="12" t="b">
         <v>1</v>
@@ -3012,44 +3072,46 @@
       <c r="M11" s="12" t="b">
         <v>1</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" s="12">
         <v>150</v>
       </c>
-      <c r="O11" s="12" t="s">
+      <c r="P11" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="12" t="s">
+      <c r="R11" s="12"/>
+      <c r="S11" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="S11" s="12">
+      <c r="T11" s="12">
         <v>500</v>
       </c>
-      <c r="T11" s="12" t="s">
+      <c r="U11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="U11" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="V11" s="12">
-        <v>1</v>
-      </c>
-      <c r="W11" s="12"/>
+      <c r="V11" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W11" s="12">
+        <v>1</v>
+      </c>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12"/>
-      <c r="AB11" s="12" t="b">
-        <v>1</v>
-      </c>
+      <c r="AB11" s="12"/>
       <c r="AC11" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="AD11" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="12"/>
+        <v>1</v>
+      </c>
+      <c r="AD11" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="b">
+        <v>0</v>
+      </c>
       <c r="AF11" s="12"/>
       <c r="AG11" s="12"/>
       <c r="AH11" s="12"/>
@@ -3062,8 +3124,9 @@
       <c r="AO11" s="12"/>
       <c r="AP11" s="12"/>
       <c r="AQ11" s="12"/>
-    </row>
-    <row r="12" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AR11" s="12"/>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3091,12 +3154,12 @@
       <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="J12" t="str">
+      <c r="J12" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K12" t="b">
-        <v>1</v>
+      <c r="K12" t="s">
+        <v>169</v>
       </c>
       <c r="L12" t="b">
         <v>1</v>
@@ -3104,41 +3167,44 @@
       <c r="M12" t="b">
         <v>1</v>
       </c>
-      <c r="N12">
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+      <c r="O12">
         <v>150</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>55</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>74</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>20000</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>65</v>
       </c>
-      <c r="U12" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12">
-        <v>1</v>
-      </c>
-      <c r="AB12" t="b">
+      <c r="V12" t="b">
+        <v>1</v>
+      </c>
+      <c r="W12">
         <v>1</v>
       </c>
       <c r="AC12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD12" t="b">
         <v>0</v>
       </c>
-      <c r="AQ12">
+      <c r="AE12" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR12">
         <v>19.7</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3166,54 +3232,57 @@
       <c r="I13" t="b">
         <v>1</v>
       </c>
-      <c r="J13" t="str">
+      <c r="J13" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K13" t="b">
-        <v>0</v>
+      <c r="K13" t="s">
+        <v>168</v>
       </c>
       <c r="L13" t="b">
         <v>0</v>
       </c>
-      <c r="AB13" t="b">
+      <c r="M13" t="b">
         <v>0</v>
       </c>
       <c r="AC13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF13" t="s">
         <v>86</v>
       </c>
-      <c r="AF13">
+      <c r="AG13">
         <v>60</v>
       </c>
-      <c r="AG13" t="s">
+      <c r="AH13" t="s">
         <v>65</v>
       </c>
-      <c r="AH13" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL13" t="s">
+      <c r="AI13" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM13" t="s">
         <v>52</v>
       </c>
-      <c r="AM13">
+      <c r="AN13">
         <v>10</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AO13" t="s">
         <v>53</v>
       </c>
-      <c r="AO13" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AP13" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3241,53 +3310,56 @@
       <c r="I14" t="b">
         <v>1</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="K14" t="b">
-        <v>0</v>
+      <c r="K14" t="s">
+        <v>168</v>
       </c>
       <c r="L14" t="b">
         <v>0</v>
       </c>
-      <c r="AB14" t="b">
+      <c r="M14" t="b">
         <v>0</v>
       </c>
       <c r="AC14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF14" t="s">
         <v>86</v>
       </c>
-      <c r="AF14">
+      <c r="AG14">
         <v>80</v>
       </c>
-      <c r="AG14" t="s">
+      <c r="AH14" t="s">
         <v>65</v>
       </c>
-      <c r="AH14" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL14" t="s">
+      <c r="AI14" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM14" t="s">
         <v>52</v>
       </c>
-      <c r="AM14">
+      <c r="AN14">
         <v>10</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AO14" t="s">
         <v>53</v>
       </c>
-      <c r="AO14" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AP14" t="b">
+        <v>1</v>
+      </c>
+      <c r="AQ14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -3315,54 +3387,57 @@
       <c r="I15" t="b">
         <v>1</v>
       </c>
-      <c r="J15" t="str">
+      <c r="J15" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K15" t="b">
-        <v>0</v>
+      <c r="K15" t="s">
+        <v>168</v>
       </c>
       <c r="L15" t="b">
         <v>0</v>
       </c>
-      <c r="AB15" t="b">
+      <c r="M15" t="b">
         <v>0</v>
       </c>
       <c r="AC15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF15" t="s">
         <v>86</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>60</v>
       </c>
-      <c r="AG15" t="s">
+      <c r="AH15" t="s">
         <v>65</v>
       </c>
-      <c r="AH15" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL15" t="s">
+      <c r="AI15" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM15" t="s">
         <v>52</v>
       </c>
-      <c r="AM15">
+      <c r="AN15">
         <v>10</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AO15" t="s">
         <v>53</v>
       </c>
-      <c r="AO15" t="b">
-        <v>1</v>
-      </c>
-      <c r="AQ15">
+      <c r="AP15" t="b">
+        <v>1</v>
+      </c>
+      <c r="AR15">
         <v>10.8</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -3390,11 +3465,11 @@
       <c r="I16" t="b">
         <v>0</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="K16" t="b">
-        <v>1</v>
+      <c r="K16" t="s">
+        <v>169</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
@@ -3402,41 +3477,44 @@
       <c r="M16" t="b">
         <v>1</v>
       </c>
-      <c r="N16">
+      <c r="N16" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16">
         <v>150</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>55</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>200</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>55</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>96</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>100</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>65</v>
       </c>
-      <c r="U16" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB16" t="b">
-        <v>1</v>
+      <c r="V16" t="b">
+        <v>0</v>
       </c>
       <c r="AC16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AE16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -3464,12 +3542,12 @@
       <c r="I17" t="b">
         <v>0</v>
       </c>
-      <c r="J17" t="str">
+      <c r="J17" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K17" t="b">
-        <v>1</v>
+      <c r="K17" t="s">
+        <v>169</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
@@ -3477,41 +3555,44 @@
       <c r="M17" t="b">
         <v>1</v>
       </c>
-      <c r="N17">
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17">
         <v>150</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>55</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>200</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>55</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>96</v>
       </c>
-      <c r="S17">
+      <c r="T17">
         <v>100</v>
       </c>
-      <c r="T17" t="s">
+      <c r="U17" t="s">
         <v>65</v>
       </c>
-      <c r="U17" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB17" t="b">
-        <v>1</v>
+      <c r="V17" t="b">
+        <v>0</v>
       </c>
       <c r="AC17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AE17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -3539,12 +3620,12 @@
       <c r="I18" t="b">
         <v>0</v>
       </c>
-      <c r="J18" t="str">
+      <c r="J18" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K18" t="b">
-        <v>1</v>
+      <c r="K18" t="s">
+        <v>169</v>
       </c>
       <c r="L18" t="b">
         <v>1</v>
@@ -3552,41 +3633,44 @@
       <c r="M18" t="b">
         <v>1</v>
       </c>
-      <c r="N18">
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18">
         <v>150</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>55</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>200</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>55</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" t="s">
         <v>96</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>150</v>
       </c>
-      <c r="T18" t="s">
+      <c r="U18" t="s">
         <v>65</v>
       </c>
-      <c r="U18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB18" t="b">
-        <v>1</v>
+      <c r="V18" t="b">
+        <v>0</v>
       </c>
       <c r="AC18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AE18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -3614,11 +3698,11 @@
       <c r="I19" t="b">
         <v>0</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="K19" t="b">
-        <v>1</v>
+      <c r="K19" t="s">
+        <v>169</v>
       </c>
       <c r="L19" t="b">
         <v>1</v>
@@ -3626,44 +3710,47 @@
       <c r="M19" t="b">
         <v>1</v>
       </c>
-      <c r="N19">
+      <c r="N19" t="b">
+        <v>1</v>
+      </c>
+      <c r="O19">
         <v>150</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>55</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>200</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>55</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>96</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>150</v>
       </c>
-      <c r="T19" t="s">
+      <c r="U19" t="s">
         <v>65</v>
       </c>
-      <c r="U19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB19" t="b">
-        <v>1</v>
+      <c r="V19" t="b">
+        <v>0</v>
       </c>
       <c r="AC19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19" t="b">
         <v>0</v>
       </c>
-      <c r="AQ19">
+      <c r="AE19" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR19">
         <v>15.6</v>
       </c>
     </row>
-    <row r="20" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -3691,12 +3778,12 @@
       <c r="I20" t="b">
         <v>0</v>
       </c>
-      <c r="J20" t="str">
+      <c r="J20" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K20" t="b">
-        <v>1</v>
+      <c r="K20" t="s">
+        <v>169</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
@@ -3704,44 +3791,47 @@
       <c r="M20" t="b">
         <v>1</v>
       </c>
-      <c r="N20">
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+      <c r="O20">
         <v>150</v>
       </c>
-      <c r="O20" t="s">
+      <c r="P20" t="s">
         <v>55</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>200</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>55</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" t="s">
         <v>101</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>150</v>
       </c>
-      <c r="T20" t="s">
+      <c r="U20" t="s">
         <v>65</v>
       </c>
-      <c r="U20" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB20" t="b">
-        <v>1</v>
+      <c r="V20" t="b">
+        <v>0</v>
       </c>
       <c r="AC20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD20" t="b">
         <v>0</v>
       </c>
-      <c r="AQ20">
+      <c r="AE20" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR20">
         <v>19.3</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -3769,12 +3859,13 @@
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="J21" t="str">
+      <c r="J21" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K21" t="b">
-        <v>1</v>
+      <c r="K21" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
@@ -3782,17 +3873,20 @@
       <c r="M21" t="b">
         <v>1</v>
       </c>
-      <c r="AB21" t="b">
+      <c r="N21" t="b">
         <v>1</v>
       </c>
       <c r="AC21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AE21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -3820,12 +3914,13 @@
       <c r="I22" t="b">
         <v>1</v>
       </c>
-      <c r="J22" t="str">
+      <c r="J22" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K22" t="b">
-        <v>1</v>
+      <c r="K22" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -3833,17 +3928,20 @@
       <c r="M22" t="b">
         <v>1</v>
       </c>
-      <c r="AB22" t="b">
+      <c r="N22" t="b">
         <v>1</v>
       </c>
       <c r="AC22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AE22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -3871,12 +3969,13 @@
       <c r="I23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" t="str">
+      <c r="J23" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K23" t="b">
-        <v>1</v>
+      <c r="K23" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L23" t="b">
         <v>1</v>
@@ -3884,20 +3983,23 @@
       <c r="M23" t="b">
         <v>1</v>
       </c>
-      <c r="AB23" t="b">
+      <c r="N23" t="b">
         <v>1</v>
       </c>
       <c r="AC23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD23" t="b">
         <v>0</v>
       </c>
-      <c r="AQ23">
+      <c r="AE23" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR23">
         <v>15.6</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>13</v>
       </c>
@@ -3925,57 +4027,60 @@
       <c r="I24" t="b">
         <v>1</v>
       </c>
-      <c r="J24" t="str">
+      <c r="J24" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K24" t="b">
-        <v>0</v>
+      <c r="K24" t="s">
+        <v>168</v>
       </c>
       <c r="L24" t="b">
         <v>0</v>
       </c>
-      <c r="AB24" t="b">
+      <c r="M24" t="b">
         <v>0</v>
       </c>
       <c r="AC24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF24" t="s">
         <v>52</v>
       </c>
-      <c r="AF24">
+      <c r="AG24">
         <v>10</v>
       </c>
-      <c r="AG24" t="s">
+      <c r="AH24" t="s">
         <v>53</v>
       </c>
-      <c r="AH24" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI24">
-        <v>1</v>
-      </c>
-      <c r="AL24" t="s">
+      <c r="AI24" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ24">
+        <v>1</v>
+      </c>
+      <c r="AM24" t="s">
         <v>62</v>
       </c>
-      <c r="AM24">
+      <c r="AN24">
         <v>50</v>
       </c>
-      <c r="AN24" t="s">
+      <c r="AO24" t="s">
         <v>55</v>
       </c>
-      <c r="AO24" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ24">
+      <c r="AP24" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR24">
         <v>12.6</v>
       </c>
     </row>
-    <row r="25" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -4003,57 +4108,60 @@
       <c r="I25" t="b">
         <v>1</v>
       </c>
-      <c r="J25" t="str">
+      <c r="J25" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K25" t="b">
-        <v>0</v>
+      <c r="K25" t="s">
+        <v>168</v>
       </c>
       <c r="L25" t="b">
         <v>0</v>
       </c>
-      <c r="AB25" t="b">
+      <c r="M25" t="b">
         <v>0</v>
       </c>
       <c r="AC25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD25" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF25" t="s">
         <v>52</v>
       </c>
-      <c r="AF25">
+      <c r="AG25">
         <v>10</v>
       </c>
-      <c r="AG25" t="s">
+      <c r="AH25" t="s">
         <v>53</v>
       </c>
-      <c r="AH25" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI25">
-        <v>1</v>
-      </c>
-      <c r="AL25" t="s">
+      <c r="AI25" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ25">
+        <v>1</v>
+      </c>
+      <c r="AM25" t="s">
         <v>111</v>
       </c>
-      <c r="AM25">
+      <c r="AN25">
         <v>50</v>
       </c>
-      <c r="AN25" t="s">
+      <c r="AO25" t="s">
         <v>55</v>
       </c>
-      <c r="AO25" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ25">
+      <c r="AP25" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR25">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -4081,12 +4189,12 @@
       <c r="I26" t="b">
         <v>1</v>
       </c>
-      <c r="J26" t="str">
+      <c r="J26" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K26" t="b">
-        <v>1</v>
+      <c r="K26" t="s">
+        <v>169</v>
       </c>
       <c r="L26" t="b">
         <v>1</v>
@@ -4094,17 +4202,20 @@
       <c r="M26" t="b">
         <v>1</v>
       </c>
-      <c r="AB26" t="b">
+      <c r="N26" t="b">
         <v>1</v>
       </c>
       <c r="AC26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AE26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -4132,12 +4243,12 @@
       <c r="I27" t="b">
         <v>0</v>
       </c>
-      <c r="J27" t="str">
+      <c r="J27" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K27" t="b">
-        <v>1</v>
+      <c r="K27" t="s">
+        <v>168</v>
       </c>
       <c r="L27" t="b">
         <v>1</v>
@@ -4145,23 +4256,26 @@
       <c r="M27" t="b">
         <v>1</v>
       </c>
-      <c r="N27">
+      <c r="N27" t="b">
+        <v>1</v>
+      </c>
+      <c r="O27">
         <v>75</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>55</v>
       </c>
-      <c r="AB27" t="b">
-        <v>1</v>
-      </c>
       <c r="AC27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AE27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8</v>
       </c>
@@ -4189,11 +4303,11 @@
       <c r="I28" t="b">
         <v>0</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="K28" t="b">
-        <v>1</v>
+      <c r="K28" t="s">
+        <v>167</v>
       </c>
       <c r="L28" t="b">
         <v>1</v>
@@ -4201,32 +4315,35 @@
       <c r="M28" t="b">
         <v>1</v>
       </c>
-      <c r="N28">
+      <c r="N28" t="b">
+        <v>1</v>
+      </c>
+      <c r="O28">
         <v>150</v>
       </c>
-      <c r="O28" t="s">
+      <c r="P28" t="s">
         <v>55</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>200</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>55</v>
       </c>
-      <c r="AB28" t="b">
-        <v>1</v>
-      </c>
       <c r="AC28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD28" t="b">
         <v>0</v>
       </c>
-      <c r="AQ28">
+      <c r="AE28" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR28">
         <v>13.17</v>
       </c>
     </row>
-    <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8</v>
       </c>
@@ -4254,11 +4371,11 @@
       <c r="I29" t="b">
         <v>0</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="K29" t="b">
-        <v>1</v>
+      <c r="K29" t="s">
+        <v>168</v>
       </c>
       <c r="L29" t="b">
         <v>1</v>
@@ -4266,32 +4383,35 @@
       <c r="M29" t="b">
         <v>1</v>
       </c>
-      <c r="N29">
+      <c r="N29" t="b">
+        <v>1</v>
+      </c>
+      <c r="O29">
         <v>150</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" t="s">
         <v>55</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <v>200</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>55</v>
       </c>
-      <c r="AB29" t="b">
-        <v>1</v>
-      </c>
       <c r="AC29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD29" t="b">
         <v>0</v>
       </c>
-      <c r="AQ29">
+      <c r="AE29" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR29">
         <v>17.579999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>14</v>
       </c>
@@ -4319,16 +4439,16 @@
       <c r="I30" t="b">
         <v>0</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="K30" t="b">
-        <v>0</v>
+      <c r="K30" t="s">
+        <v>169</v>
       </c>
       <c r="L30" t="b">
         <v>0</v>
       </c>
-      <c r="AB30" t="b">
+      <c r="M30" t="b">
         <v>0</v>
       </c>
       <c r="AC30" t="b">
@@ -4337,32 +4457,35 @@
       <c r="AD30" t="b">
         <v>0</v>
       </c>
-      <c r="AE30" t="s">
+      <c r="AE30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF30" t="s">
         <v>124</v>
       </c>
-      <c r="AF30">
+      <c r="AG30">
         <v>600</v>
       </c>
-      <c r="AG30" t="s">
+      <c r="AH30" t="s">
         <v>65</v>
       </c>
-      <c r="AH30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL30" t="s">
+      <c r="AI30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM30" t="s">
         <v>125</v>
       </c>
-      <c r="AM30">
+      <c r="AN30">
         <v>1000</v>
       </c>
-      <c r="AN30" t="s">
+      <c r="AO30" t="s">
         <v>65</v>
       </c>
-      <c r="AO30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AP30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>14</v>
       </c>
@@ -4390,16 +4513,16 @@
       <c r="I31" t="b">
         <v>0</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J31" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="K31" t="b">
-        <v>0</v>
+      <c r="K31" t="s">
+        <v>169</v>
       </c>
       <c r="L31" t="b">
         <v>0</v>
       </c>
-      <c r="AB31" t="b">
+      <c r="M31" t="b">
         <v>0</v>
       </c>
       <c r="AC31" t="b">
@@ -4408,20 +4531,23 @@
       <c r="AD31" t="b">
         <v>0</v>
       </c>
-      <c r="AE31" t="s">
+      <c r="AE31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF31" t="s">
         <v>125</v>
       </c>
-      <c r="AF31">
+      <c r="AG31">
         <v>1500</v>
       </c>
-      <c r="AG31" t="s">
+      <c r="AH31" t="s">
         <v>65</v>
       </c>
-      <c r="AH31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AI31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -4449,12 +4575,12 @@
       <c r="I32" t="b">
         <v>1</v>
       </c>
-      <c r="J32" t="str">
+      <c r="J32" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K32" t="b">
-        <v>1</v>
+      <c r="K32" t="s">
+        <v>167</v>
       </c>
       <c r="L32" t="b">
         <v>1</v>
@@ -4462,41 +4588,44 @@
       <c r="M32" t="b">
         <v>1</v>
       </c>
-      <c r="N32">
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32">
         <v>75</v>
       </c>
-      <c r="O32" t="s">
+      <c r="P32" t="s">
         <v>55</v>
       </c>
-      <c r="R32" t="s">
+      <c r="S32" t="s">
         <v>101</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <v>10</v>
       </c>
-      <c r="T32" t="s">
+      <c r="U32" t="s">
         <v>53</v>
       </c>
-      <c r="U32" t="b">
-        <v>1</v>
-      </c>
-      <c r="V32">
-        <v>1</v>
-      </c>
-      <c r="AB32" t="b">
+      <c r="V32" t="b">
+        <v>1</v>
+      </c>
+      <c r="W32">
         <v>1</v>
       </c>
       <c r="AC32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD32" t="b">
         <v>0</v>
       </c>
-      <c r="AQ32">
+      <c r="AE32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR32">
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -4524,12 +4653,12 @@
       <c r="I33" t="b">
         <v>1</v>
       </c>
-      <c r="J33" t="str">
+      <c r="J33" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K33" t="b">
-        <v>1</v>
+      <c r="K33" t="s">
+        <v>167</v>
       </c>
       <c r="L33" t="b">
         <v>1</v>
@@ -4537,41 +4666,44 @@
       <c r="M33" t="b">
         <v>1</v>
       </c>
-      <c r="N33">
+      <c r="N33" t="b">
+        <v>1</v>
+      </c>
+      <c r="O33">
         <v>75</v>
       </c>
-      <c r="O33" t="s">
+      <c r="P33" t="s">
         <v>55</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>52</v>
       </c>
-      <c r="S33">
+      <c r="T33">
         <v>10</v>
       </c>
-      <c r="T33" t="s">
+      <c r="U33" t="s">
         <v>53</v>
       </c>
-      <c r="U33" t="b">
-        <v>1</v>
-      </c>
-      <c r="V33">
-        <v>1</v>
-      </c>
-      <c r="AB33" t="b">
+      <c r="V33" t="b">
+        <v>1</v>
+      </c>
+      <c r="W33">
         <v>1</v>
       </c>
       <c r="AC33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD33" t="b">
         <v>0</v>
       </c>
-      <c r="AQ33">
+      <c r="AE33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR33">
         <v>15.7</v>
       </c>
     </row>
-    <row r="34" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15</v>
       </c>
@@ -4599,63 +4731,66 @@
       <c r="I34" t="b">
         <v>1</v>
       </c>
-      <c r="J34" t="str">
+      <c r="J34" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K34" t="b">
-        <v>0</v>
+      <c r="K34" t="s">
+        <v>167</v>
       </c>
       <c r="L34" t="b">
         <v>0</v>
       </c>
-      <c r="AB34" t="b">
+      <c r="M34" t="b">
         <v>0</v>
       </c>
       <c r="AC34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD34" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF34" t="s">
         <v>138</v>
       </c>
-      <c r="AF34">
+      <c r="AG34">
         <v>0.4</v>
       </c>
-      <c r="AG34" t="s">
+      <c r="AH34" t="s">
         <v>139</v>
       </c>
-      <c r="AH34" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK34">
+      <c r="AI34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK34" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL34">
         <v>0.5</v>
       </c>
-      <c r="AL34" t="s">
+      <c r="AM34" t="s">
         <v>52</v>
       </c>
-      <c r="AM34">
+      <c r="AN34">
         <v>10</v>
       </c>
-      <c r="AN34" t="s">
+      <c r="AO34" t="s">
         <v>53</v>
       </c>
-      <c r="AO34" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP34">
+      <c r="AP34" t="b">
         <v>1</v>
       </c>
       <c r="AQ34">
+        <v>1</v>
+      </c>
+      <c r="AR34">
         <v>6.6</v>
       </c>
     </row>
-    <row r="35" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15</v>
       </c>
@@ -4683,63 +4818,66 @@
       <c r="I35" t="b">
         <v>1</v>
       </c>
-      <c r="J35" t="str">
+      <c r="J35" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K35" t="b">
-        <v>0</v>
+      <c r="K35" t="s">
+        <v>167</v>
       </c>
       <c r="L35" t="b">
         <v>0</v>
       </c>
-      <c r="AB35" t="b">
+      <c r="M35" t="b">
         <v>0</v>
       </c>
       <c r="AC35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD35" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF35" t="s">
         <v>138</v>
       </c>
-      <c r="AF35">
+      <c r="AG35">
         <v>0.4</v>
       </c>
-      <c r="AG35" t="s">
+      <c r="AH35" t="s">
         <v>139</v>
       </c>
-      <c r="AH35" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ35" t="b">
-        <v>1</v>
-      </c>
-      <c r="AK35">
+      <c r="AI35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AK35" t="b">
+        <v>1</v>
+      </c>
+      <c r="AL35">
         <v>0.5</v>
       </c>
-      <c r="AL35" t="s">
+      <c r="AM35" t="s">
         <v>52</v>
       </c>
-      <c r="AM35">
+      <c r="AN35">
         <v>10</v>
       </c>
-      <c r="AN35" t="s">
+      <c r="AO35" t="s">
         <v>53</v>
       </c>
-      <c r="AO35" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP35">
+      <c r="AP35" t="b">
         <v>1</v>
       </c>
       <c r="AQ35">
+        <v>1</v>
+      </c>
+      <c r="AR35">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="36" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15</v>
       </c>
@@ -4767,45 +4905,49 @@
       <c r="I36" t="b">
         <v>1</v>
       </c>
-      <c r="J36" t="str">
+      <c r="J36" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K36" t="b">
-        <v>0</v>
+      <c r="K36" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L36" t="b">
         <v>0</v>
       </c>
-      <c r="AB36" t="b">
+      <c r="M36" t="b">
         <v>0</v>
       </c>
       <c r="AC36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD36" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE36" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF36" t="s">
         <v>52</v>
       </c>
-      <c r="AF36">
+      <c r="AG36">
         <v>10</v>
       </c>
-      <c r="AG36" t="s">
+      <c r="AH36" t="s">
         <v>53</v>
       </c>
-      <c r="AH36" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI36">
-        <v>1</v>
-      </c>
-      <c r="AQ36">
+      <c r="AI36" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ36">
+        <v>1</v>
+      </c>
+      <c r="AR36">
         <v>10.7</v>
       </c>
     </row>
-    <row r="37" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16</v>
       </c>
@@ -4833,51 +4975,55 @@
       <c r="I37" t="b">
         <v>0</v>
       </c>
-      <c r="J37" t="str">
+      <c r="J37" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K37" t="b">
-        <v>0</v>
+      <c r="K37" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L37" t="b">
         <v>0</v>
       </c>
-      <c r="AB37" t="b">
+      <c r="M37" t="b">
         <v>0</v>
       </c>
       <c r="AC37" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF37" t="s">
         <v>144</v>
       </c>
-      <c r="AF37">
+      <c r="AG37">
         <v>20</v>
       </c>
-      <c r="AG37" t="s">
+      <c r="AH37" t="s">
         <v>65</v>
       </c>
-      <c r="AH37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL37" t="s">
+      <c r="AI37" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM37" t="s">
         <v>62</v>
       </c>
-      <c r="AM37">
+      <c r="AN37">
         <v>60</v>
       </c>
-      <c r="AN37" t="s">
+      <c r="AO37" t="s">
         <v>65</v>
       </c>
-      <c r="AO37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AP37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
@@ -4905,51 +5051,55 @@
       <c r="I38" t="b">
         <v>0</v>
       </c>
-      <c r="J38" t="str">
+      <c r="J38" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K38" t="b">
-        <v>0</v>
+      <c r="K38" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L38" t="b">
         <v>0</v>
       </c>
-      <c r="AB38" t="b">
+      <c r="M38" t="b">
         <v>0</v>
       </c>
       <c r="AC38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD38" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE38" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF38" t="s">
         <v>144</v>
       </c>
-      <c r="AF38">
+      <c r="AG38">
         <v>40</v>
       </c>
-      <c r="AG38" t="s">
+      <c r="AH38" t="s">
         <v>65</v>
       </c>
-      <c r="AH38" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL38" t="s">
+      <c r="AI38" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM38" t="s">
         <v>62</v>
       </c>
-      <c r="AM38">
+      <c r="AN38">
         <v>60</v>
       </c>
-      <c r="AN38" t="s">
+      <c r="AO38" t="s">
         <v>65</v>
       </c>
-      <c r="AO38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AP38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>16</v>
       </c>
@@ -4977,51 +5127,54 @@
       <c r="I39" t="b">
         <v>0</v>
       </c>
-      <c r="J39" t="str">
+      <c r="J39" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K39" t="b">
-        <v>0</v>
+      <c r="K39" t="s">
+        <v>168</v>
       </c>
       <c r="L39" t="b">
         <v>0</v>
       </c>
-      <c r="AB39" t="b">
+      <c r="M39" t="b">
         <v>0</v>
       </c>
       <c r="AC39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE39" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF39" t="s">
         <v>144</v>
       </c>
-      <c r="AF39">
+      <c r="AG39">
         <v>40</v>
       </c>
-      <c r="AG39" t="s">
+      <c r="AH39" t="s">
         <v>65</v>
       </c>
-      <c r="AH39" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL39" t="s">
+      <c r="AI39" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM39" t="s">
         <v>62</v>
       </c>
-      <c r="AM39">
+      <c r="AN39">
         <v>75</v>
       </c>
-      <c r="AN39" t="s">
+      <c r="AO39" t="s">
         <v>65</v>
       </c>
-      <c r="AO39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AP39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>16</v>
       </c>
@@ -5049,54 +5202,58 @@
       <c r="I40" t="b">
         <v>0</v>
       </c>
-      <c r="J40" t="str">
+      <c r="J40" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K40" t="b">
-        <v>0</v>
+      <c r="K40" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L40" t="b">
         <v>0</v>
       </c>
-      <c r="AB40" t="b">
+      <c r="M40" t="b">
         <v>0</v>
       </c>
       <c r="AC40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE40" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF40" t="s">
         <v>144</v>
       </c>
-      <c r="AF40">
+      <c r="AG40">
         <v>40</v>
       </c>
-      <c r="AG40" t="s">
+      <c r="AH40" t="s">
         <v>65</v>
       </c>
-      <c r="AH40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL40" t="s">
+      <c r="AI40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM40" t="s">
         <v>62</v>
       </c>
-      <c r="AM40">
+      <c r="AN40">
         <v>75</v>
       </c>
-      <c r="AN40" t="s">
+      <c r="AO40" t="s">
         <v>65</v>
       </c>
-      <c r="AO40" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ40">
+      <c r="AP40" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR40">
         <v>10.3</v>
       </c>
     </row>
-    <row r="41" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>16</v>
       </c>
@@ -5124,54 +5281,58 @@
       <c r="I41" t="b">
         <v>0</v>
       </c>
-      <c r="J41" t="str">
+      <c r="J41" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K41" t="b">
-        <v>0</v>
+      <c r="K41" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L41" t="b">
         <v>0</v>
       </c>
-      <c r="AB41" t="b">
+      <c r="M41" t="b">
         <v>0</v>
       </c>
       <c r="AC41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD41" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE41" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF41" t="s">
         <v>144</v>
       </c>
-      <c r="AF41">
+      <c r="AG41">
         <v>40</v>
       </c>
-      <c r="AG41" t="s">
+      <c r="AH41" t="s">
         <v>65</v>
       </c>
-      <c r="AH41" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL41" t="s">
+      <c r="AI41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM41" t="s">
         <v>62</v>
       </c>
-      <c r="AM41">
+      <c r="AN41">
         <v>150</v>
       </c>
-      <c r="AN41" t="s">
+      <c r="AO41" t="s">
         <v>65</v>
       </c>
-      <c r="AO41" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ41">
+      <c r="AP41" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR41">
         <v>10.7</v>
       </c>
     </row>
-    <row r="42" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>16</v>
       </c>
@@ -5199,54 +5360,58 @@
       <c r="I42" t="b">
         <v>0</v>
       </c>
-      <c r="J42" t="str">
+      <c r="J42" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K42" t="b">
-        <v>0</v>
+      <c r="K42" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L42" t="b">
         <v>0</v>
       </c>
-      <c r="AB42" t="b">
+      <c r="M42" t="b">
         <v>0</v>
       </c>
       <c r="AC42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD42" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE42" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF42" t="s">
         <v>144</v>
       </c>
-      <c r="AF42">
+      <c r="AG42">
         <v>40</v>
       </c>
-      <c r="AG42" t="s">
+      <c r="AH42" t="s">
         <v>65</v>
       </c>
-      <c r="AH42" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL42" t="s">
+      <c r="AI42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM42" t="s">
         <v>62</v>
       </c>
-      <c r="AM42">
+      <c r="AN42">
         <v>75</v>
       </c>
-      <c r="AN42" t="s">
+      <c r="AO42" t="s">
         <v>65</v>
       </c>
-      <c r="AO42" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ42">
+      <c r="AP42" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR42">
         <v>4.7</v>
       </c>
     </row>
-    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -5274,12 +5439,13 @@
       <c r="I43" t="b">
         <v>0</v>
       </c>
-      <c r="J43" t="str">
+      <c r="J43" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K43" t="b">
-        <v>1</v>
+      <c r="K43" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L43" t="b">
         <v>1</v>
@@ -5287,35 +5453,38 @@
       <c r="M43" t="b">
         <v>1</v>
       </c>
-      <c r="N43">
+      <c r="N43" t="b">
+        <v>1</v>
+      </c>
+      <c r="O43">
         <v>150</v>
       </c>
-      <c r="O43" t="s">
+      <c r="P43" t="s">
         <v>55</v>
       </c>
-      <c r="R43" t="s">
+      <c r="S43" t="s">
         <v>154</v>
       </c>
-      <c r="S43">
+      <c r="T43">
         <v>500</v>
       </c>
-      <c r="T43" t="s">
+      <c r="U43" t="s">
         <v>65</v>
       </c>
-      <c r="U43" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB43" t="b">
-        <v>1</v>
+      <c r="V43" t="b">
+        <v>0</v>
       </c>
       <c r="AC43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AE43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -5343,12 +5512,13 @@
       <c r="I44" t="b">
         <v>0</v>
       </c>
-      <c r="J44" t="str">
+      <c r="J44" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K44" t="b">
-        <v>1</v>
+      <c r="K44" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L44" t="b">
         <v>1</v>
@@ -5356,35 +5526,38 @@
       <c r="M44" t="b">
         <v>1</v>
       </c>
-      <c r="N44">
+      <c r="N44" t="b">
+        <v>1</v>
+      </c>
+      <c r="O44">
         <v>150</v>
       </c>
-      <c r="O44" t="s">
+      <c r="P44" t="s">
         <v>55</v>
       </c>
-      <c r="R44" t="s">
+      <c r="S44" t="s">
         <v>154</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <v>500</v>
       </c>
-      <c r="T44" t="s">
+      <c r="U44" t="s">
         <v>65</v>
       </c>
-      <c r="U44" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB44" t="b">
-        <v>1</v>
+      <c r="V44" t="b">
+        <v>0</v>
       </c>
       <c r="AC44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AE44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -5412,12 +5585,13 @@
       <c r="I45" t="b">
         <v>0</v>
       </c>
-      <c r="J45" t="str">
+      <c r="J45" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K45" t="b">
-        <v>1</v>
+      <c r="K45" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>High</v>
       </c>
       <c r="L45" t="b">
         <v>1</v>
@@ -5425,35 +5599,38 @@
       <c r="M45" t="b">
         <v>1</v>
       </c>
-      <c r="N45">
+      <c r="N45" t="b">
+        <v>1</v>
+      </c>
+      <c r="O45">
         <v>150</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>55</v>
       </c>
-      <c r="R45" t="s">
+      <c r="S45" t="s">
         <v>154</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <v>400</v>
       </c>
-      <c r="T45" t="s">
+      <c r="U45" t="s">
         <v>65</v>
       </c>
-      <c r="U45" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB45" t="b">
-        <v>1</v>
+      <c r="V45" t="b">
+        <v>0</v>
       </c>
       <c r="AC45" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AE45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>16</v>
       </c>
@@ -5481,51 +5658,54 @@
       <c r="I46" t="b">
         <v>0</v>
       </c>
-      <c r="J46" t="str">
+      <c r="J46" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K46" t="b">
-        <v>0</v>
+      <c r="K46" t="s">
+        <v>168</v>
       </c>
       <c r="L46" t="b">
         <v>0</v>
       </c>
-      <c r="AB46" t="b">
+      <c r="M46" t="b">
         <v>0</v>
       </c>
       <c r="AC46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD46" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE46" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF46" t="s">
         <v>144</v>
       </c>
-      <c r="AF46">
+      <c r="AG46">
         <v>20</v>
       </c>
-      <c r="AG46" t="s">
+      <c r="AH46" t="s">
         <v>65</v>
       </c>
-      <c r="AH46" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL46" t="s">
+      <c r="AI46" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM46" t="s">
         <v>62</v>
       </c>
-      <c r="AM46">
+      <c r="AN46">
         <v>75</v>
       </c>
-      <c r="AN46" t="s">
+      <c r="AO46" t="s">
         <v>65</v>
       </c>
-      <c r="AO46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AP46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>16</v>
       </c>
@@ -5553,50 +5733,54 @@
       <c r="I47" t="b">
         <v>0</v>
       </c>
-      <c r="J47" t="str">
+      <c r="J47" s="25" t="str">
         <f>IF(OR(Table2[[#This Row],[% Serious AE]] &lt; 0.2, Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR(Table2[[#This Row],[% Serious AE]] &gt;= 0.5, Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC(Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K47" t="b">
-        <v>0</v>
+      <c r="K47" t="str">
+        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+        <v>Medium</v>
       </c>
       <c r="L47" t="b">
         <v>0</v>
       </c>
-      <c r="AB47" t="b">
+      <c r="M47" t="b">
         <v>0</v>
       </c>
       <c r="AC47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD47" t="b">
-        <v>0</v>
-      </c>
-      <c r="AE47" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF47" t="s">
         <v>144</v>
       </c>
-      <c r="AF47">
+      <c r="AG47">
         <v>40</v>
       </c>
-      <c r="AG47" t="s">
+      <c r="AH47" t="s">
         <v>65</v>
       </c>
-      <c r="AH47" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL47" t="s">
+      <c r="AI47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM47" t="s">
         <v>62</v>
       </c>
-      <c r="AM47">
+      <c r="AN47">
         <v>150</v>
       </c>
-      <c r="AN47" t="s">
+      <c r="AO47" t="s">
         <v>65</v>
       </c>
-      <c r="AO47" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ47">
+      <c r="AP47" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR47">
         <v>4.7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Burden & Dropout Reasons
</commit_message>
<xml_diff>
--- a/variable-dosing_7119.xlsx
+++ b/variable-dosing_7119.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beaston\Desktop\GBM-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4923BEC5-A01E-487F-8EA7-A2A117D4EBED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3FD21B34-6619-4FAE-9DE1-7E42F973D950}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studies" sheetId="2" r:id="rId1"/>
@@ -20,9 +20,6 @@
     <sheet name="Concomitant" sheetId="6" r:id="rId5"/>
     <sheet name="Concomitant Tem" sheetId="7" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="988" uniqueCount="187">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1004" uniqueCount="187">
   <si>
     <t>Phase</t>
   </si>
@@ -1230,7 +1227,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1274,6 +1271,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1557,31 +1557,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Studies"/>
-      <sheetName val="Arms"/>
-      <sheetName val="Dropout"/>
-      <sheetName val="Neoadjuvant"/>
-      <sheetName val="Concomitant"/>
-      <sheetName val="Concomitant Tem"/>
-      <sheetName val="Burden Rank"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2222,8 +2197,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2304,7 +2279,7 @@
       <c r="J1" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="27" t="s">
         <v>170</v>
       </c>
       <c r="L1" s="8" t="s">
@@ -2436,11 +2411,11 @@
         <v>1</v>
       </c>
       <c r="J2" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K2" t="s">
-        <v>169</v>
+      <c r="K2" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -2522,11 +2497,11 @@
       <c r="I3" t="b">
         <v>0</v>
       </c>
-      <c r="J3" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Low</v>
+      </c>
+      <c r="K3" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L3" t="b">
@@ -2585,11 +2560,11 @@
       <c r="I4" t="b">
         <v>0</v>
       </c>
-      <c r="J4" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J4" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="26" t="s">
         <v>169</v>
       </c>
       <c r="L4" s="11" t="b">
@@ -2674,11 +2649,11 @@
       <c r="I5" t="b">
         <v>0</v>
       </c>
-      <c r="J5" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J5" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="26" t="s">
         <v>169</v>
       </c>
       <c r="L5" s="11" t="b">
@@ -2752,11 +2727,11 @@
       <c r="I6" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J6" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="26" t="s">
         <v>169</v>
       </c>
       <c r="L6" s="11" t="b">
@@ -2830,13 +2805,12 @@
       <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J7" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K7" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="K7" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L7" s="11" t="b">
         <v>0</v>
@@ -2900,12 +2874,12 @@
       <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="J8" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J8" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K8" t="s">
-        <v>167</v>
+      <c r="K8" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L8" s="11" t="b">
         <v>0</v>
@@ -2969,13 +2943,12 @@
       <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="J9" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J9" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K9" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="K9" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
@@ -3048,13 +3021,12 @@
       <c r="I10" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K10" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
+      <c r="J10" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
@@ -3112,12 +3084,12 @@
       <c r="I11" t="b">
         <v>1</v>
       </c>
-      <c r="J11" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J11" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K11" t="s">
-        <v>169</v>
+      <c r="K11" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L11" s="12" t="b">
         <v>1</v>
@@ -3207,12 +3179,12 @@
       <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="J12" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J12" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K12" t="s">
-        <v>169</v>
+      <c r="K12" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L12" t="b">
         <v>1</v>
@@ -3285,11 +3257,11 @@
       <c r="I13" t="b">
         <v>1</v>
       </c>
-      <c r="J13" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J13" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L13" t="b">
@@ -3363,11 +3335,11 @@
       <c r="I14" t="b">
         <v>1</v>
       </c>
-      <c r="J14" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J14" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L14" t="b">
@@ -3441,11 +3413,11 @@
       <c r="I15" t="b">
         <v>1</v>
       </c>
-      <c r="J15" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J15" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L15" t="b">
@@ -3519,12 +3491,12 @@
       <c r="I16" t="b">
         <v>0</v>
       </c>
-      <c r="J16" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K16" t="s">
-        <v>169</v>
+      <c r="J16" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K16" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
@@ -3597,12 +3569,12 @@
       <c r="I17" t="b">
         <v>0</v>
       </c>
-      <c r="J17" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K17" t="s">
-        <v>169</v>
+      <c r="J17" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K17" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
@@ -3675,12 +3647,12 @@
       <c r="I18" t="b">
         <v>0</v>
       </c>
-      <c r="J18" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K18" t="s">
-        <v>169</v>
+      <c r="J18" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L18" t="b">
         <v>1</v>
@@ -3753,12 +3725,12 @@
       <c r="I19" t="b">
         <v>0</v>
       </c>
-      <c r="J19" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K19" t="s">
-        <v>169</v>
+      <c r="J19" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L19" t="b">
         <v>1</v>
@@ -3834,12 +3806,12 @@
       <c r="I20" t="b">
         <v>0</v>
       </c>
-      <c r="J20" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K20" t="s">
-        <v>169</v>
+      <c r="J20" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K20" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
@@ -3915,13 +3887,12 @@
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="J21" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J21" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K21" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="K21" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
@@ -3970,13 +3941,12 @@
       <c r="I22" t="b">
         <v>1</v>
       </c>
-      <c r="J22" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J22" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K22" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="K22" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -4025,13 +3995,12 @@
       <c r="I23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J23" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K23" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="K23" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L23" t="b">
         <v>1</v>
@@ -4083,11 +4052,11 @@
       <c r="I24" t="b">
         <v>1</v>
       </c>
-      <c r="J24" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J24" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L24" t="b">
@@ -4164,11 +4133,11 @@
       <c r="I25" t="b">
         <v>1</v>
       </c>
-      <c r="J25" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J25" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L25" t="b">
@@ -4245,12 +4214,12 @@
       <c r="I26" t="b">
         <v>1</v>
       </c>
-      <c r="J26" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J26" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K26" t="s">
-        <v>169</v>
+      <c r="K26" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L26" t="b">
         <v>1</v>
@@ -4299,11 +4268,11 @@
       <c r="I27" t="b">
         <v>0</v>
       </c>
-      <c r="J27" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="J27" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K27" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L27" t="b">
@@ -4359,11 +4328,11 @@
       <c r="I28" t="b">
         <v>0</v>
       </c>
-      <c r="J28" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J28" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="26" t="s">
         <v>167</v>
       </c>
       <c r="L28" t="b">
@@ -4428,11 +4397,11 @@
       <c r="I29" t="b">
         <v>0</v>
       </c>
-      <c r="J29" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J29" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K29" s="26" t="s">
         <v>168</v>
       </c>
       <c r="L29" t="b">
@@ -4497,11 +4466,11 @@
       <c r="I30" t="b">
         <v>0</v>
       </c>
-      <c r="J30" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J30" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K30" s="26" t="s">
         <v>169</v>
       </c>
       <c r="L30" t="b">
@@ -4572,11 +4541,11 @@
       <c r="I31" t="b">
         <v>0</v>
       </c>
-      <c r="J31" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J31" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K31" s="26" t="s">
         <v>169</v>
       </c>
       <c r="L31" t="b">
@@ -4635,11 +4604,11 @@
       <c r="I32" t="b">
         <v>1</v>
       </c>
-      <c r="J32" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J32" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K32" t="s">
+      <c r="K32" s="26" t="s">
         <v>167</v>
       </c>
       <c r="L32" t="b">
@@ -4713,11 +4682,11 @@
       <c r="I33" t="b">
         <v>1</v>
       </c>
-      <c r="J33" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J33" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>High</v>
       </c>
-      <c r="K33" t="s">
+      <c r="K33" s="26" t="s">
         <v>167</v>
       </c>
       <c r="L33" t="b">
@@ -4791,12 +4760,12 @@
       <c r="I34" t="b">
         <v>1</v>
       </c>
-      <c r="J34" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J34" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K34" t="s">
-        <v>167</v>
+      <c r="K34" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L34" t="b">
         <v>0</v>
@@ -4878,12 +4847,12 @@
       <c r="I35" t="b">
         <v>1</v>
       </c>
-      <c r="J35" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J35" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K35" t="s">
-        <v>167</v>
+      <c r="K35" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="L35" t="b">
         <v>0</v>
@@ -4965,13 +4934,12 @@
       <c r="I36" t="b">
         <v>1</v>
       </c>
-      <c r="J36" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J36" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Medium</v>
       </c>
-      <c r="K36" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>Medium</v>
+      <c r="K36" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L36" t="b">
         <v>0</v>
@@ -5035,13 +5003,12 @@
       <c r="I37" t="b">
         <v>0</v>
       </c>
-      <c r="J37" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J37" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K37" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>Medium</v>
+      <c r="K37" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L37" t="b">
         <v>0</v>
@@ -5111,13 +5078,12 @@
       <c r="I38" t="b">
         <v>0</v>
       </c>
-      <c r="J38" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J38" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K38" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>Medium</v>
+      <c r="K38" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L38" t="b">
         <v>0</v>
@@ -5187,12 +5153,12 @@
       <c r="I39" t="b">
         <v>0</v>
       </c>
-      <c r="J39" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J39" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K39" t="s">
-        <v>168</v>
+      <c r="K39" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L39" t="b">
         <v>0</v>
@@ -5262,13 +5228,12 @@
       <c r="I40" t="b">
         <v>0</v>
       </c>
-      <c r="J40" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J40" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K40" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>Medium</v>
+      <c r="K40" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L40" t="b">
         <v>0</v>
@@ -5341,13 +5306,12 @@
       <c r="I41" t="b">
         <v>0</v>
       </c>
-      <c r="J41" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J41" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K41" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>Medium</v>
+      <c r="K41" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L41" t="b">
         <v>0</v>
@@ -5420,13 +5384,12 @@
       <c r="I42" t="b">
         <v>0</v>
       </c>
-      <c r="J42" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J42" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K42" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>Medium</v>
+      <c r="K42" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L42" t="b">
         <v>0</v>
@@ -5499,13 +5462,12 @@
       <c r="I43" t="b">
         <v>0</v>
       </c>
-      <c r="J43" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K43" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="J43" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K43" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L43" t="b">
         <v>1</v>
@@ -5572,13 +5534,12 @@
       <c r="I44" t="b">
         <v>0</v>
       </c>
-      <c r="J44" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K44" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="J44" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K44" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L44" t="b">
         <v>1</v>
@@ -5645,13 +5606,12 @@
       <c r="I45" t="b">
         <v>0</v>
       </c>
-      <c r="J45" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
-        <v>High</v>
-      </c>
-      <c r="K45" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>High</v>
+      <c r="J45" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+        <v>Medium</v>
+      </c>
+      <c r="K45" s="26" t="s">
+        <v>167</v>
       </c>
       <c r="L45" t="b">
         <v>1</v>
@@ -5718,12 +5678,12 @@
       <c r="I46" t="b">
         <v>0</v>
       </c>
-      <c r="J46" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J46" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K46" t="s">
-        <v>168</v>
+      <c r="K46" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L46" t="b">
         <v>0</v>
@@ -5793,13 +5753,12 @@
       <c r="I47" t="b">
         <v>0</v>
       </c>
-      <c r="J47" s="25" t="str">
-        <f>IF(OR(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), AND(Table2[[#This Row],[Concomitant]] = TRUE, Table2[[#This Row],[Adjuvant]] = TRUE)), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
+      <c r="J47" s="28" t="str">
+        <f>IF(OR(AND(Table2[[#This Row],[Radiation]] = TRUE, Table2[[#This Row],[Universal IV]] = TRUE), Table2[[#This Row],[Surgery]] = TRUE), "High",  IF(AND(Table2[[#This Row],[Radiation]] = FALSE, Table2[[#This Row],[Universal IV]] = FALSE), "Low", "Medium"))</f>
         <v>Low</v>
       </c>
-      <c r="K47" t="str">
-        <f>IF(OR([1]!Table2[[#This Row],[% Serious AE]] &lt; 0.2, [1]!Table2[[#This Row],[% Non Serious AE]] &lt; 0.25  ), "Low", IF(OR([1]!Table2[[#This Row],[% Serious AE]] &gt;= 0.5, [1]!Table2[[#This Row],[% Non Serious AE]] &gt;= _xlfn.PERCENTILE.INC([1]!Table2[% Non Serious AE], 0.66)),  "High", "Medium"))</f>
-        <v>Medium</v>
+      <c r="K47" s="26" t="s">
+        <v>169</v>
       </c>
       <c r="L47" t="b">
         <v>0</v>
@@ -5858,7 +5817,7 @@
   <dimension ref="A1:D166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8655,7 +8614,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADA338F0-BFD0-4788-963F-7C359787317C}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>